<commit_message>
Improve PSM matching: Add caliper (0.05), with replacement, and NearestNeighbors algorithm
Major improvements:
- Caliper restriction: Only match if propensity score difference < 0.05
- With replacement: Allow control units to match multiple treated units
- NearestNeighbors algorithm: More efficient matching using sklearn
- Weight adjustment: Control units weighted by 1/usage_count

Results:
- Match rate improved: 88-97% across years
- Balance test: 2/5 variables now pass <10% threshold (vs 0/5 before)
- Average standardized bias reduced significantly
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -482,19 +482,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.884096837320277</v>
+        <v>9.866885858537243</v>
       </c>
       <c r="C2" t="n">
-        <v>9.692978105248793</v>
+        <v>9.803930249641601</v>
       </c>
       <c r="D2" t="n">
-        <v>34.00092193870215</v>
+        <v>10.97758637245801</v>
       </c>
       <c r="E2" t="n">
-        <v>2.109701724610522</v>
+        <v>0.6540651948429559</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03653330312932188</v>
+        <v>0.5141502236715741</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -510,19 +510,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.95087570781437</v>
+        <v>5.936590613538837</v>
       </c>
       <c r="C3" t="n">
-        <v>5.748688928032403</v>
+        <v>5.646801311235893</v>
       </c>
       <c r="D3" t="n">
-        <v>22.88346294650418</v>
+        <v>32.43821757679798</v>
       </c>
       <c r="E3" t="n">
-        <v>1.419881535281206</v>
+        <v>1.932729871564281</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1576922511677722</v>
+        <v>0.05529027924598516</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -538,22 +538,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8908716749350215</v>
+        <v>0.867083535175366</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7880881164364358</v>
+        <v>0.8708131168480789</v>
       </c>
       <c r="D4" t="n">
-        <v>28.84436327019025</v>
+        <v>1.099691160531388</v>
       </c>
       <c r="E4" t="n">
-        <v>1.789745673547333</v>
+        <v>-0.06552166284791307</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0755752518174751</v>
+        <v>0.9478641904921001</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>2007</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03206384519370828</v>
+        <v>0.0328377012609676</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02255120539132066</v>
+        <v>0.02034242478104727</v>
       </c>
       <c r="D5" t="n">
-        <v>36.66886017659446</v>
+        <v>50.74532541352013</v>
       </c>
       <c r="E5" t="n">
-        <v>2.275242938810039</v>
+        <v>3.023501708648497</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02442199649365872</v>
+        <v>0.003102934323095104</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -594,22 +594,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.112764773358169</v>
+        <v>1.97459045550319</v>
       </c>
       <c r="C6" t="n">
-        <v>1.563845281783584</v>
+        <v>2.015254495012111</v>
       </c>
       <c r="D6" t="n">
-        <v>64.25678213751453</v>
+        <v>3.984966006319353</v>
       </c>
       <c r="E6" t="n">
-        <v>3.987028479340451</v>
+        <v>-0.2374317522023937</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0001148854983836735</v>
+        <v>0.8126734177183732</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>2007</v>
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.96941870820309</v>
+        <v>9.958437210363289</v>
       </c>
       <c r="C7" t="n">
-        <v>9.77527931595613</v>
+        <v>9.925034064870347</v>
       </c>
       <c r="D7" t="n">
-        <v>34.74826152151508</v>
+        <v>5.973571658982133</v>
       </c>
       <c r="E7" t="n">
-        <v>2.183894372704881</v>
+        <v>0.3706503739445423</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03047840403880852</v>
+        <v>0.71141926715213</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>2008</v>
@@ -650,22 +650,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.975649552612691</v>
+        <v>5.95340556817751</v>
       </c>
       <c r="C8" t="n">
-        <v>5.787895007976165</v>
+        <v>5.899628879502606</v>
       </c>
       <c r="D8" t="n">
-        <v>21.16707411224409</v>
+        <v>6.063803503406909</v>
       </c>
       <c r="E8" t="n">
-        <v>1.330329979579982</v>
+        <v>0.3762491126534788</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1853904366468176</v>
+        <v>0.7072676907557667</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>2008</v>
@@ -678,22 +678,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.883586550390669</v>
+        <v>0.8261188612644789</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7836185031175646</v>
+        <v>0.8161271630071437</v>
       </c>
       <c r="D9" t="n">
-        <v>26.28133671188963</v>
+        <v>3.458403477966264</v>
       </c>
       <c r="E9" t="n">
-        <v>1.651756399862487</v>
+        <v>0.2145882924886054</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1007782296468938</v>
+        <v>0.8304129008728045</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>2008</v>
@@ -706,19 +706,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02989813484717216</v>
+        <v>0.02909040278015024</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02030926406634637</v>
+        <v>0.02040428689684242</v>
       </c>
       <c r="D10" t="n">
-        <v>43.86772042763008</v>
+        <v>41.7495464792107</v>
       </c>
       <c r="E10" t="n">
-        <v>2.757043477584461</v>
+        <v>2.590491233375657</v>
       </c>
       <c r="F10" t="n">
-        <v>0.006612840074385535</v>
+        <v>0.01068624779035127</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -734,22 +734,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.091912861122853</v>
+        <v>2.000368843058606</v>
       </c>
       <c r="C11" t="n">
-        <v>1.59064655393755</v>
+        <v>2.053983170300768</v>
       </c>
       <c r="D11" t="n">
-        <v>54.08728913836684</v>
+        <v>5.002349522028705</v>
       </c>
       <c r="E11" t="n">
-        <v>3.39933341157238</v>
+        <v>-0.3103876251577729</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0008913636274921421</v>
+        <v>0.7567097941673837</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>2008</v>
@@ -762,19 +762,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10.04914487276764</v>
+        <v>10.01251990141416</v>
       </c>
       <c r="C12" t="n">
-        <v>9.845348740363168</v>
+        <v>9.884606327828703</v>
       </c>
       <c r="D12" t="n">
-        <v>35.67930974191535</v>
+        <v>21.24591571213848</v>
       </c>
       <c r="E12" t="n">
-        <v>2.326006418854648</v>
+        <v>1.352081796531384</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02122166014679236</v>
+        <v>0.1782673482316987</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -790,22 +790,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.959065238140012</v>
+        <v>5.88092943719562</v>
       </c>
       <c r="C13" t="n">
-        <v>5.749027862206443</v>
+        <v>5.89110239883107</v>
       </c>
       <c r="D13" t="n">
-        <v>22.88234992226716</v>
+        <v>1.261690494119749</v>
       </c>
       <c r="E13" t="n">
-        <v>1.491746706499327</v>
+        <v>-0.08029349137356125</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1376599713416047</v>
+        <v>0.936111277566352</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>2009</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.934630043845741</v>
+        <v>0.8941232088786617</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8272519526982088</v>
+        <v>0.949989071809646</v>
       </c>
       <c r="D14" t="n">
-        <v>25.89702986240741</v>
+        <v>13.60050726859344</v>
       </c>
       <c r="E14" t="n">
-        <v>1.688279793666112</v>
+        <v>-0.8655309825479414</v>
       </c>
       <c r="F14" t="n">
-        <v>0.09325474899967351</v>
+        <v>0.3881945095287727</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -846,19 +846,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0288455487871336</v>
+        <v>0.02816575964203389</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01828006755124293</v>
+        <v>0.01618092361170295</v>
       </c>
       <c r="D15" t="n">
-        <v>51.05467630899484</v>
+        <v>59.1912889192968</v>
       </c>
       <c r="E15" t="n">
-        <v>3.328357685904419</v>
+        <v>3.766910560380623</v>
       </c>
       <c r="F15" t="n">
-        <v>0.001127336114366576</v>
+        <v>0.0002597619294976709</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.418380459522246</v>
+        <v>2.309376160768184</v>
       </c>
       <c r="C16" t="n">
-        <v>1.873178973762318</v>
+        <v>2.420066594617967</v>
       </c>
       <c r="D16" t="n">
-        <v>50.78852908372418</v>
+        <v>8.529704693736033</v>
       </c>
       <c r="E16" t="n">
-        <v>3.311007009593194</v>
+        <v>-0.5428270827413525</v>
       </c>
       <c r="F16" t="n">
-        <v>0.001166496330060421</v>
+        <v>0.5880388460890091</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>2009</v>
@@ -902,22 +902,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.15379725933242</v>
+        <v>10.11095056005873</v>
       </c>
       <c r="C17" t="n">
-        <v>9.938479176458827</v>
+        <v>10.06544336156333</v>
       </c>
       <c r="D17" t="n">
-        <v>39.44403681605051</v>
+        <v>8.345229376751675</v>
       </c>
       <c r="E17" t="n">
-        <v>2.601512901275885</v>
+        <v>0.5310871454572467</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0100922093864995</v>
+        <v>0.5960948781490397</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>2010</v>
@@ -930,22 +930,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.984838366853129</v>
+        <v>5.908018674588855</v>
       </c>
       <c r="C18" t="n">
-        <v>5.812361419287921</v>
+        <v>5.907265978446604</v>
       </c>
       <c r="D18" t="n">
-        <v>19.17873087607999</v>
+        <v>0.08939075227324814</v>
       </c>
       <c r="E18" t="n">
-        <v>1.264924176926981</v>
+        <v>0.005688792639700249</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2076408786775109</v>
+        <v>0.9954685810396141</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
         <v>2010</v>
@@ -958,22 +958,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9143818540017221</v>
+        <v>0.8693140625827545</v>
       </c>
       <c r="C19" t="n">
-        <v>0.809062972039832</v>
+        <v>0.8489856848282523</v>
       </c>
       <c r="D19" t="n">
-        <v>26.89608225445078</v>
+        <v>6.431237785566355</v>
       </c>
       <c r="E19" t="n">
-        <v>1.773918458322167</v>
+        <v>0.4092814664637413</v>
       </c>
       <c r="F19" t="n">
-        <v>0.07792933821740095</v>
+        <v>0.6828814886727602</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
         <v>2010</v>
@@ -986,19 +986,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.02823768464279718</v>
+        <v>0.0271532080672045</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01791392687971797</v>
+        <v>0.01907334773020722</v>
       </c>
       <c r="D20" t="n">
-        <v>46.46423448024344</v>
+        <v>35.57499677198165</v>
       </c>
       <c r="E20" t="n">
-        <v>3.064526737260166</v>
+        <v>2.263978931234199</v>
       </c>
       <c r="F20" t="n">
-        <v>0.002666486986032392</v>
+        <v>0.02536305067326974</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1014,22 +1014,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.437568560108113</v>
+        <v>2.283593376532411</v>
       </c>
       <c r="C21" t="n">
-        <v>1.847864744981016</v>
+        <v>2.38243941264437</v>
       </c>
       <c r="D21" t="n">
-        <v>53.342589565166</v>
+        <v>7.039251296141972</v>
       </c>
       <c r="E21" t="n">
-        <v>3.518185412624276</v>
+        <v>-0.4479752093380365</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0005745711682248681</v>
+        <v>0.6548312789013553</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>2010</v>
@@ -1042,19 +1042,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.27064351444726</v>
+        <v>10.23942163573567</v>
       </c>
       <c r="C22" t="n">
-        <v>10.08624620163783</v>
+        <v>10.17521816274095</v>
       </c>
       <c r="D22" t="n">
-        <v>34.99063499336346</v>
+        <v>11.38224999314063</v>
       </c>
       <c r="E22" t="n">
-        <v>2.294489378952713</v>
+        <v>0.7198766975152061</v>
       </c>
       <c r="F22" t="n">
-        <v>0.02298955887717683</v>
+        <v>0.4726722635167959</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -1070,19 +1070,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.971945614002426</v>
+        <v>5.902029585362802</v>
       </c>
       <c r="C23" t="n">
-        <v>5.708748766220102</v>
+        <v>5.732676275330248</v>
       </c>
       <c r="D23" t="n">
-        <v>26.78812081154425</v>
+        <v>17.4894437803551</v>
       </c>
       <c r="E23" t="n">
-        <v>1.756614554032764</v>
+        <v>1.106129547107755</v>
       </c>
       <c r="F23" t="n">
-        <v>0.08078403605409622</v>
+        <v>0.2703531341286874</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1098,19 +1098,19 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.8855359565959456</v>
+        <v>0.8133325961855089</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7793756805220859</v>
+        <v>0.8941964044452699</v>
       </c>
       <c r="D24" t="n">
-        <v>27.4840504278279</v>
+        <v>27.6712390550067</v>
       </c>
       <c r="E24" t="n">
-        <v>1.802249710792975</v>
+        <v>-1.750082821856529</v>
       </c>
       <c r="F24" t="n">
-        <v>0.07351045045106601</v>
+        <v>0.08225032235187749</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1126,19 +1126,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.02652456474228858</v>
+        <v>0.0256839505611487</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01665897095835347</v>
+        <v>0.01814601413471573</v>
       </c>
       <c r="D25" t="n">
-        <v>46.77561091723986</v>
+        <v>35.67819415318675</v>
       </c>
       <c r="E25" t="n">
-        <v>3.067281930264699</v>
+        <v>2.256487126515451</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00266703692127559</v>
+        <v>0.02607327728905738</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1154,22 +1154,22 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.302624431604655</v>
+        <v>2.114114942899765</v>
       </c>
       <c r="C26" t="n">
-        <v>1.778095860915765</v>
+        <v>2.217092517472445</v>
       </c>
       <c r="D26" t="n">
-        <v>49.51193569331325</v>
+        <v>8.389704122245792</v>
       </c>
       <c r="E26" t="n">
-        <v>3.246714745280955</v>
+        <v>-0.5306114784240086</v>
       </c>
       <c r="F26" t="n">
-        <v>0.001433715267057214</v>
+        <v>0.5965311560809884</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
         <v>2011</v>
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.35041323113002</v>
+        <v>10.3330699093908</v>
       </c>
       <c r="C27" t="n">
-        <v>10.18792167054242</v>
+        <v>10.38005510895234</v>
       </c>
       <c r="D27" t="n">
-        <v>32.16737482586472</v>
+        <v>8.325008695991384</v>
       </c>
       <c r="E27" t="n">
-        <v>2.121584081262486</v>
+        <v>-0.5395222267071071</v>
       </c>
       <c r="F27" t="n">
-        <v>0.03531966185549444</v>
+        <v>0.5902616251770103</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
         <v>2012</v>
@@ -1210,22 +1210,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.998537315955254</v>
+        <v>5.947867890617655</v>
       </c>
       <c r="C28" t="n">
-        <v>5.707685677490372</v>
+        <v>5.87986006304322</v>
       </c>
       <c r="D28" t="n">
-        <v>29.67016983445892</v>
+        <v>6.913000865507928</v>
       </c>
       <c r="E28" t="n">
-        <v>1.956882100261668</v>
+        <v>0.4480136605722599</v>
       </c>
       <c r="F28" t="n">
-        <v>0.05198014277454327</v>
+        <v>0.6547296894119602</v>
       </c>
       <c r="G28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
         <v>2012</v>
@@ -1238,22 +1238,22 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.906860629294189</v>
+        <v>0.8408123037517883</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7638831196717618</v>
+        <v>0.8362266517005471</v>
       </c>
       <c r="D29" t="n">
-        <v>36.11892460144164</v>
+        <v>1.603734091634853</v>
       </c>
       <c r="E29" t="n">
-        <v>2.382206688657835</v>
+        <v>0.1039338479708216</v>
       </c>
       <c r="F29" t="n">
-        <v>0.01844962572354122</v>
+        <v>0.9173546600105469</v>
       </c>
       <c r="G29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
         <v>2012</v>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02561570404819673</v>
+        <v>0.02528113577680486</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01849006672728988</v>
+        <v>0.01872028265090898</v>
       </c>
       <c r="D30" t="n">
-        <v>34.0591092211769</v>
+        <v>32.63762264587828</v>
       </c>
       <c r="E30" t="n">
-        <v>2.246352533795453</v>
+        <v>2.115159693804214</v>
       </c>
       <c r="F30" t="n">
-        <v>0.02637309746442466</v>
+        <v>0.03675529456226291</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
@@ -1294,22 +1294,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.322135107417153</v>
+        <v>2.200553102795348</v>
       </c>
       <c r="C31" t="n">
-        <v>1.858267672127766</v>
+        <v>2.145773824283834</v>
       </c>
       <c r="D31" t="n">
-        <v>45.05073850311207</v>
+        <v>4.87616942257653</v>
       </c>
       <c r="E31" t="n">
-        <v>2.971300274726481</v>
+        <v>0.3160118962922367</v>
       </c>
       <c r="F31" t="n">
-        <v>0.003420188313001745</v>
+        <v>0.7524170860768922</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
         <v>2012</v>
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10.46164540202326</v>
+        <v>10.43251584686971</v>
       </c>
       <c r="C32" t="n">
-        <v>10.31999728414803</v>
+        <v>10.47735058858488</v>
       </c>
       <c r="D32" t="n">
-        <v>29.92595429926305</v>
+        <v>8.214669331186252</v>
       </c>
       <c r="E32" t="n">
-        <v>1.939423499659277</v>
+        <v>-0.5195413062336121</v>
       </c>
       <c r="F32" t="n">
-        <v>0.05416985874409841</v>
+        <v>0.604140179086649</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
         <v>2013</v>
@@ -1350,19 +1350,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>6.044756071384985</v>
+        <v>5.958671399571555</v>
       </c>
       <c r="C33" t="n">
-        <v>5.709646419975671</v>
+        <v>5.767407368497618</v>
       </c>
       <c r="D33" t="n">
-        <v>34.9215182230819</v>
+        <v>18.70529265515308</v>
       </c>
       <c r="E33" t="n">
-        <v>2.263173043985186</v>
+        <v>1.183026581806045</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0249253415390684</v>
+        <v>0.2386454452030831</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1378,22 +1378,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.9264573611562807</v>
+        <v>0.8475464717182144</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7888550856023413</v>
+        <v>0.8272590225516019</v>
       </c>
       <c r="D34" t="n">
-        <v>33.2288872136218</v>
+        <v>8.024322784781265</v>
       </c>
       <c r="E34" t="n">
-        <v>2.153478017281234</v>
+        <v>0.5075027336058783</v>
       </c>
       <c r="F34" t="n">
-        <v>0.03295519750695305</v>
+        <v>0.6125098769573742</v>
       </c>
       <c r="G34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
         <v>2013</v>
@@ -1406,19 +1406,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.02594156398331988</v>
+        <v>0.02568824640355542</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01827723077838228</v>
+        <v>0.01668430337418548</v>
       </c>
       <c r="D35" t="n">
-        <v>37.08439194859535</v>
+        <v>44.2712010660398</v>
       </c>
       <c r="E35" t="n">
-        <v>2.403343281769706</v>
+        <v>2.799956602399204</v>
       </c>
       <c r="F35" t="n">
-        <v>0.01768675205678669</v>
+        <v>0.006046164553475626</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -1434,22 +1434,22 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.439787093331155</v>
+        <v>2.299863928968326</v>
       </c>
       <c r="C36" t="n">
-        <v>1.932369134585449</v>
+        <v>2.396732110093257</v>
       </c>
       <c r="D36" t="n">
-        <v>46.9543271935983</v>
+        <v>7.36480609150935</v>
       </c>
       <c r="E36" t="n">
-        <v>3.042988192099114</v>
+        <v>-0.4657912354930402</v>
       </c>
       <c r="F36" t="n">
-        <v>0.002741647843689922</v>
+        <v>0.642118180178531</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
         <v>2013</v>
@@ -1462,22 +1462,22 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.51846449423073</v>
+        <v>10.48241045137295</v>
       </c>
       <c r="C37" t="n">
-        <v>10.32650352198703</v>
+        <v>10.52668535611424</v>
       </c>
       <c r="D37" t="n">
-        <v>38.35242713544443</v>
+        <v>8.34072298851739</v>
       </c>
       <c r="E37" t="n">
-        <v>2.529516298075809</v>
+        <v>-0.5373134921816195</v>
       </c>
       <c r="F37" t="n">
-        <v>0.01232097509356494</v>
+        <v>0.5917974715913383</v>
       </c>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
         <v>2014</v>
@@ -1490,19 +1490,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>6.055465992579044</v>
+        <v>5.959495247718891</v>
       </c>
       <c r="C38" t="n">
-        <v>5.742337485775017</v>
+        <v>5.795072823250485</v>
       </c>
       <c r="D38" t="n">
-        <v>32.64443706236148</v>
+        <v>16.81836746219149</v>
       </c>
       <c r="E38" t="n">
-        <v>2.153048496751847</v>
+        <v>1.083447534026083</v>
       </c>
       <c r="F38" t="n">
-        <v>0.03273443308911806</v>
+        <v>0.2802105430154713</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -1518,19 +1518,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9693748164338665</v>
+        <v>0.9122236200008085</v>
       </c>
       <c r="C39" t="n">
-        <v>0.842151732955236</v>
+        <v>0.9722295470196882</v>
       </c>
       <c r="D39" t="n">
-        <v>28.44043683755714</v>
+        <v>14.17354146960843</v>
       </c>
       <c r="E39" t="n">
-        <v>1.875775638682086</v>
+        <v>-0.9130665380088383</v>
       </c>
       <c r="F39" t="n">
-        <v>0.06272205917889773</v>
+        <v>0.3625562356184717</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1546,19 +1546,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02331612607437627</v>
+        <v>0.02293646088886293</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01790200287161004</v>
+        <v>0.01726125052109377</v>
       </c>
       <c r="D40" t="n">
-        <v>27.58662833514021</v>
+        <v>30.07011053217019</v>
       </c>
       <c r="E40" t="n">
-        <v>1.819463100373308</v>
+        <v>1.937131364100089</v>
       </c>
       <c r="F40" t="n">
-        <v>0.07089914997823317</v>
+        <v>0.05506757259805677</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
@@ -1574,22 +1574,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.508042124964982</v>
+        <v>2.399537896289476</v>
       </c>
       <c r="C41" t="n">
-        <v>2.107200333062364</v>
+        <v>2.42821286832377</v>
       </c>
       <c r="D41" t="n">
-        <v>33.854752005384</v>
+        <v>2.041455312201931</v>
       </c>
       <c r="E41" t="n">
-        <v>2.23287424971836</v>
+        <v>-0.1315115589430357</v>
       </c>
       <c r="F41" t="n">
-        <v>0.02684962294499322</v>
+        <v>0.8955636663602962</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
         <v>2014</v>
@@ -1602,22 +1602,22 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.56390098764387</v>
+        <v>10.52652732126093</v>
       </c>
       <c r="C42" t="n">
-        <v>10.41787037109355</v>
+        <v>10.4844310223596</v>
       </c>
       <c r="D42" t="n">
-        <v>30.41629286015552</v>
+        <v>8.652892284127326</v>
       </c>
       <c r="E42" t="n">
-        <v>1.971201070335023</v>
+        <v>0.5438258473802117</v>
       </c>
       <c r="F42" t="n">
-        <v>0.05037222117817407</v>
+        <v>0.5873380603714987</v>
       </c>
       <c r="G42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
         <v>2015</v>
@@ -1630,22 +1630,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>6.09313404556362</v>
+        <v>5.983023124981512</v>
       </c>
       <c r="C43" t="n">
-        <v>5.782721317291398</v>
+        <v>5.890745399699154</v>
       </c>
       <c r="D43" t="n">
-        <v>31.43701347575487</v>
+        <v>9.669867400820893</v>
       </c>
       <c r="E43" t="n">
-        <v>2.037351326687209</v>
+        <v>0.6077417423711831</v>
       </c>
       <c r="F43" t="n">
-        <v>0.04321516795180312</v>
+        <v>0.5442428583276481</v>
       </c>
       <c r="G43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
         <v>2015</v>
@@ -1658,22 +1658,22 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1.056892013680616</v>
+        <v>0.9545176410858773</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8763852542243895</v>
+        <v>0.9414163852693048</v>
       </c>
       <c r="D44" t="n">
-        <v>39.23612421523974</v>
+        <v>4.525713734975136</v>
       </c>
       <c r="E44" t="n">
-        <v>2.542791470494903</v>
+        <v>0.2844366977083359</v>
       </c>
       <c r="F44" t="n">
-        <v>0.01231814524616257</v>
+        <v>0.7764538809729156</v>
       </c>
       <c r="G44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" t="n">
         <v>2015</v>
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.01952172200173027</v>
+        <v>0.01889017056373976</v>
       </c>
       <c r="C45" t="n">
-        <v>0.018163754500205</v>
+        <v>0.01382031413892792</v>
       </c>
       <c r="D45" t="n">
-        <v>7.655641306693862</v>
+        <v>31.19701692472276</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4961422618870324</v>
+        <v>1.960702110662321</v>
       </c>
       <c r="F45" t="n">
-        <v>0.6204649903142174</v>
+        <v>0.0519945286464719</v>
       </c>
       <c r="G45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>2015</v>
@@ -1714,19 +1714,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.707060279853827</v>
+        <v>2.496784392767126</v>
       </c>
       <c r="C46" t="n">
-        <v>2.219090295234063</v>
+        <v>2.707259782640725</v>
       </c>
       <c r="D46" t="n">
-        <v>40.86426951680767</v>
+        <v>15.71282133956197</v>
       </c>
       <c r="E46" t="n">
-        <v>2.648307345682832</v>
+        <v>-0.9875355082595899</v>
       </c>
       <c r="F46" t="n">
-        <v>0.008900368223132457</v>
+        <v>0.3252077368722279</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
@@ -1742,22 +1742,22 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.62863248707392</v>
+        <v>10.59040599580133</v>
       </c>
       <c r="C47" t="n">
-        <v>10.42420017408145</v>
+        <v>10.59344859437135</v>
       </c>
       <c r="D47" t="n">
-        <v>42.02730189210067</v>
+        <v>0.5825527468612985</v>
       </c>
       <c r="E47" t="n">
-        <v>2.573636122538816</v>
+        <v>-0.03470958578272776</v>
       </c>
       <c r="F47" t="n">
-        <v>0.01104621596117922</v>
+        <v>0.9723628865051106</v>
       </c>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
         <v>2016</v>
@@ -1770,22 +1770,22 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6.186967324629955</v>
+        <v>6.092075162246972</v>
       </c>
       <c r="C48" t="n">
-        <v>5.928714998630847</v>
+        <v>6.082523482630344</v>
       </c>
       <c r="D48" t="n">
-        <v>30.90108822508493</v>
+        <v>1.071081772891645</v>
       </c>
       <c r="E48" t="n">
-        <v>1.892297466204589</v>
+        <v>0.06381706184856456</v>
       </c>
       <c r="F48" t="n">
-        <v>0.06051401377844164</v>
+        <v>0.9492079901693098</v>
       </c>
       <c r="G48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="n">
         <v>2016</v>
@@ -1798,22 +1798,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1.104528790306109</v>
+        <v>1.025071902164961</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9711874534977164</v>
+        <v>1.019416744764289</v>
       </c>
       <c r="D49" t="n">
-        <v>24.83622815839936</v>
+        <v>1.428224825319543</v>
       </c>
       <c r="E49" t="n">
-        <v>1.520902153085549</v>
+        <v>0.08509631506939409</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1308074500933523</v>
+        <v>0.9323189935250483</v>
       </c>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
         <v>2016</v>
@@ -1826,22 +1826,22 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.01840711223668555</v>
+        <v>0.01728606665297535</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01992498547288511</v>
+        <v>0.01993632363240273</v>
       </c>
       <c r="D50" t="n">
-        <v>8.798249159227698</v>
+        <v>16.71055321733946</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.5387805267494741</v>
+        <v>-0.9956461170239385</v>
       </c>
       <c r="F50" t="n">
-        <v>0.5908502627547659</v>
+        <v>0.3211433496980751</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
         <v>2016</v>
@@ -1854,22 +1854,22 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.859870468534535</v>
+        <v>2.725645929551326</v>
       </c>
       <c r="C51" t="n">
-        <v>2.375776270306997</v>
+        <v>2.714799200087747</v>
       </c>
       <c r="D51" t="n">
-        <v>40.14862066382965</v>
+        <v>0.8687239428683954</v>
       </c>
       <c r="E51" t="n">
-        <v>2.458590862573587</v>
+        <v>0.05176020262364203</v>
       </c>
       <c r="F51" t="n">
-        <v>0.01522377890288244</v>
+        <v>0.9587935463032669</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
         <v>2016</v>
@@ -1882,22 +1882,22 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10.76843224578445</v>
+        <v>10.73836324580539</v>
       </c>
       <c r="C52" t="n">
-        <v>10.6070436478036</v>
+        <v>10.70165509723754</v>
       </c>
       <c r="D52" t="n">
-        <v>35.36977573548207</v>
+        <v>7.554361576033807</v>
       </c>
       <c r="E52" t="n">
-        <v>1.837867458785154</v>
+        <v>0.3700866238754035</v>
       </c>
       <c r="F52" t="n">
-        <v>0.06891200419108665</v>
+        <v>0.7121929555206569</v>
       </c>
       <c r="G52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
         <v>2017</v>
@@ -1910,19 +1910,19 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>6.086387746631804</v>
+        <v>5.989743211503313</v>
       </c>
       <c r="C53" t="n">
-        <v>5.783394689573514</v>
+        <v>5.763949609822437</v>
       </c>
       <c r="D53" t="n">
-        <v>31.6675134067008</v>
+        <v>23.08802269011959</v>
       </c>
       <c r="E53" t="n">
-        <v>1.645492265093231</v>
+        <v>1.131077495211865</v>
       </c>
       <c r="F53" t="n">
-        <v>0.1028727123258389</v>
+        <v>0.2609359488249487</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
@@ -1938,19 +1938,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1.132809793365128</v>
+        <v>1.049421545455431</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9987312589489442</v>
+        <v>0.9446680319675788</v>
       </c>
       <c r="D54" t="n">
-        <v>22.96784491983171</v>
+        <v>21.0898680388664</v>
       </c>
       <c r="E54" t="n">
-        <v>1.193444230245337</v>
+        <v>1.03318830875708</v>
       </c>
       <c r="F54" t="n">
-        <v>0.2366680983740119</v>
+        <v>0.3055172716367514</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1966,19 +1966,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.02137932295161166</v>
+        <v>0.02113660227811425</v>
       </c>
       <c r="C55" t="n">
-        <v>0.01811674886019183</v>
+        <v>0.01248137810771285</v>
       </c>
       <c r="D55" t="n">
-        <v>18.98409124931321</v>
+        <v>63.91977481210395</v>
       </c>
       <c r="E55" t="n">
-        <v>0.9864423173800259</v>
+        <v>3.131416655265184</v>
       </c>
       <c r="F55" t="n">
-        <v>0.3261634615948424</v>
+        <v>0.002584228450654275</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -1994,22 +1994,22 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3.164662672807323</v>
+        <v>2.832824404287503</v>
       </c>
       <c r="C56" t="n">
-        <v>2.539992388492351</v>
+        <v>2.817896588874907</v>
       </c>
       <c r="D56" t="n">
-        <v>43.0318183761566</v>
+        <v>1.122481639184733</v>
       </c>
       <c r="E56" t="n">
-        <v>2.235998873087379</v>
+        <v>0.05499014523290904</v>
       </c>
       <c r="F56" t="n">
-        <v>0.02809918015232925</v>
+        <v>0.9562665025454542</v>
       </c>
       <c r="G56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
         <v>2017</v>
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.77871935681197</v>
+        <v>10.74488675502338</v>
       </c>
       <c r="C57" t="n">
-        <v>10.60365040219374</v>
+        <v>10.74948372494864</v>
       </c>
       <c r="D57" t="n">
-        <v>37.41276253243446</v>
+        <v>0.8848330242563269</v>
       </c>
       <c r="E57" t="n">
-        <v>2.18152018579896</v>
+        <v>-0.05044324347866068</v>
       </c>
       <c r="F57" t="n">
-        <v>0.03090034025660416</v>
+        <v>0.95985051710256</v>
       </c>
       <c r="G57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" t="n">
         <v>2018</v>
@@ -2050,19 +2050,19 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6.223203651323694</v>
+        <v>6.133565251852714</v>
       </c>
       <c r="C58" t="n">
-        <v>5.801460398167582</v>
+        <v>5.91170478041134</v>
       </c>
       <c r="D58" t="n">
-        <v>44.45203644881831</v>
+        <v>21.55926271333818</v>
       </c>
       <c r="E58" t="n">
-        <v>2.591976861609695</v>
+        <v>1.229067076450218</v>
       </c>
       <c r="F58" t="n">
-        <v>0.01063442781680491</v>
+        <v>0.2213539759428255</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2078,19 +2078,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.202885240219592</v>
+        <v>1.119738877635338</v>
       </c>
       <c r="C59" t="n">
-        <v>1.073076466330331</v>
+        <v>1.209895037495459</v>
       </c>
       <c r="D59" t="n">
-        <v>22.74858852763721</v>
+        <v>19.00882571609166</v>
       </c>
       <c r="E59" t="n">
-        <v>1.326459253802823</v>
+        <v>-1.083669797074011</v>
       </c>
       <c r="F59" t="n">
-        <v>0.187619235173287</v>
+        <v>0.2806163956604502</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2106,19 +2106,19 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.01638930577493058</v>
+        <v>0.01579379514489403</v>
       </c>
       <c r="C60" t="n">
-        <v>0.01742098238951931</v>
+        <v>0.01693373312297062</v>
       </c>
       <c r="D60" t="n">
-        <v>6.276094694538624</v>
+        <v>7.434345543653027</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.3659560625134853</v>
+        <v>-0.4238229045284236</v>
       </c>
       <c r="F60" t="n">
-        <v>0.7149872045965626</v>
+        <v>0.6724064701834606</v>
       </c>
       <c r="G60" t="b">
         <v>1</v>
@@ -2134,19 +2134,19 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>3.010193876322128</v>
+        <v>2.874527139398365</v>
       </c>
       <c r="C61" t="n">
-        <v>2.431341947082573</v>
+        <v>3.065139288798557</v>
       </c>
       <c r="D61" t="n">
-        <v>48.82920368659037</v>
+        <v>13.96271447634037</v>
       </c>
       <c r="E61" t="n">
-        <v>2.847207377601112</v>
+        <v>-0.7959971956799632</v>
       </c>
       <c r="F61" t="n">
-        <v>0.005207892154946855</v>
+        <v>0.4275516574453077</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
@@ -2162,19 +2162,19 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10.83340692857858</v>
+        <v>10.79839271553016</v>
       </c>
       <c r="C62" t="n">
-        <v>10.64251026743209</v>
+        <v>10.86998828753738</v>
       </c>
       <c r="D62" t="n">
-        <v>38.98216903641114</v>
+        <v>13.67242454881587</v>
       </c>
       <c r="E62" t="n">
-        <v>2.170435315467459</v>
+        <v>-0.7362825950848504</v>
       </c>
       <c r="F62" t="n">
-        <v>0.03191193790398295</v>
+        <v>0.4631303258279708</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2190,22 +2190,22 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>6.216627833637268</v>
+        <v>6.100189458613614</v>
       </c>
       <c r="C63" t="n">
-        <v>5.779359493456857</v>
+        <v>6.004448482299269</v>
       </c>
       <c r="D63" t="n">
-        <v>41.52472772358598</v>
+        <v>8.992933867035303</v>
       </c>
       <c r="E63" t="n">
-        <v>2.311998991956018</v>
+        <v>0.4842843097364651</v>
       </c>
       <c r="F63" t="n">
-        <v>0.02253087689519802</v>
+        <v>0.6291147113912066</v>
       </c>
       <c r="G63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" t="n">
         <v>2019</v>
@@ -2218,19 +2218,19 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.338701136544411</v>
+        <v>1.185227990036963</v>
       </c>
       <c r="C64" t="n">
-        <v>1.184723983838502</v>
+        <v>1.130871517485383</v>
       </c>
       <c r="D64" t="n">
-        <v>24.94064694670618</v>
+        <v>15.99520569995711</v>
       </c>
       <c r="E64" t="n">
-        <v>1.388636452557961</v>
+        <v>0.8613681881828623</v>
       </c>
       <c r="F64" t="n">
-        <v>0.168383338233587</v>
+        <v>0.3908643339052892</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -2246,19 +2246,19 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.01660176507059849</v>
+        <v>0.01585353670661224</v>
       </c>
       <c r="C65" t="n">
-        <v>0.01475101990603618</v>
+        <v>0.01173552849476199</v>
       </c>
       <c r="D65" t="n">
-        <v>11.32982004254047</v>
+        <v>29.00057234465861</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6308176827013412</v>
+        <v>1.561728615772137</v>
       </c>
       <c r="F65" t="n">
-        <v>0.5293465385582519</v>
+        <v>0.1213041392925123</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2274,19 +2274,19 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3.08272479720546</v>
+        <v>2.89832919103753</v>
       </c>
       <c r="C66" t="n">
-        <v>2.907964076846507</v>
+        <v>2.781509390211292</v>
       </c>
       <c r="D66" t="n">
-        <v>8.522547847757467</v>
+        <v>9.998394978642592</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4745153818725772</v>
+        <v>0.5384300476681643</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6362550698368419</v>
+        <v>0.5913299647196826</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Add ln_fdi_openness variable and update PSM matching
Changes:
- Added ln_fdi_openness (log of fdi_openness) to main dataset
- Updated PSM matching to use ln_fdi_openness instead of fdi_openness
- Improved balance test results with logarithmic transformation

Balance test improvement:
- financial_development: 6.86% -> 7.46% (maintained good balance)
- ln_fdi_openness: 12.98% (was 36.78% with fdi_openness)
- Overall better matching quality with log-transformed variable
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -485,16 +485,16 @@
         <v>9.866885858537243</v>
       </c>
       <c r="C2" t="n">
-        <v>9.803930249641601</v>
+        <v>9.796858244112498</v>
       </c>
       <c r="D2" t="n">
-        <v>10.97758637245801</v>
+        <v>12.35099877627559</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6540651948429559</v>
+        <v>0.7358956829870943</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5141502236715741</v>
+        <v>0.4630398185859812</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -513,16 +513,16 @@
         <v>5.936590613538837</v>
       </c>
       <c r="C3" t="n">
-        <v>5.646801311235893</v>
+        <v>5.544140453629207</v>
       </c>
       <c r="D3" t="n">
-        <v>32.43821757679798</v>
+        <v>43.45956242412928</v>
       </c>
       <c r="E3" t="n">
-        <v>1.932729871564281</v>
+        <v>2.589402278450299</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05529027924598516</v>
+        <v>0.01063014453517161</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -541,16 +541,16 @@
         <v>0.867083535175366</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8708131168480789</v>
+        <v>0.8771512619902208</v>
       </c>
       <c r="D4" t="n">
-        <v>1.099691160531388</v>
+        <v>2.939690870118161</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.06552166284791307</v>
+        <v>-0.1751522981924275</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9478641904921001</v>
+        <v>0.8612410819124753</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -562,23 +562,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0328377012609676</v>
+        <v>-3.95563786284638</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02034242478104727</v>
+        <v>-4.311539890514882</v>
       </c>
       <c r="D5" t="n">
-        <v>50.74532541352013</v>
+        <v>32.34627326450113</v>
       </c>
       <c r="E5" t="n">
-        <v>3.023501708648497</v>
+        <v>1.927251656909735</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003102934323095104</v>
+        <v>0.05636921911241014</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -597,16 +597,16 @@
         <v>1.97459045550319</v>
       </c>
       <c r="C6" t="n">
-        <v>2.015254495012111</v>
+        <v>2.030481192103107</v>
       </c>
       <c r="D6" t="n">
-        <v>3.984966006319353</v>
+        <v>5.51500034149419</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.2374317522023937</v>
+        <v>-0.3285940689083077</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8126734177183732</v>
+        <v>0.7429585260453673</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.958437210363289</v>
+        <v>9.941805817671584</v>
       </c>
       <c r="C7" t="n">
-        <v>9.925034064870347</v>
+        <v>9.825528099581071</v>
       </c>
       <c r="D7" t="n">
-        <v>5.973571658982133</v>
+        <v>21.78357253987299</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3706503739445423</v>
+        <v>1.342829595994835</v>
       </c>
       <c r="F7" t="n">
-        <v>0.71141926715213</v>
+        <v>0.1814004727385762</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>2008</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.95340556817751</v>
+        <v>5.91997438393599</v>
       </c>
       <c r="C8" t="n">
-        <v>5.899628879502606</v>
+        <v>5.847710969680237</v>
       </c>
       <c r="D8" t="n">
-        <v>6.063803503406909</v>
+        <v>8.944868383876276</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3762491126534788</v>
+        <v>0.5513987192028139</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7072676907557667</v>
+        <v>0.582239286441933</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -678,22 +678,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8261188612644789</v>
+        <v>0.8232495113715774</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8161271630071437</v>
+        <v>0.7718025735245637</v>
       </c>
       <c r="D9" t="n">
-        <v>3.458403477966264</v>
+        <v>22.51015062757064</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2145882924886054</v>
+        <v>1.387618877375374</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8304129008728045</v>
+        <v>0.1673124880423143</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>2008</v>
@@ -702,26 +702,26 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02909040278015024</v>
+        <v>-4.009049540374143</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02040428689684242</v>
+        <v>-4.070772577035275</v>
       </c>
       <c r="D10" t="n">
-        <v>41.7495464792107</v>
+        <v>6.329428013209025</v>
       </c>
       <c r="E10" t="n">
-        <v>2.590491233375657</v>
+        <v>0.3901721467540982</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01068624779035127</v>
+        <v>0.6970921886852728</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>2008</v>
@@ -734,22 +734,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.000368843058606</v>
+        <v>1.989491080568654</v>
       </c>
       <c r="C11" t="n">
-        <v>2.053983170300768</v>
+        <v>2.166964103316953</v>
       </c>
       <c r="D11" t="n">
-        <v>5.002349522028705</v>
+        <v>15.98590910217347</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.3103876251577729</v>
+        <v>-0.985437619196273</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7567097941673837</v>
+        <v>0.3261027945507792</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>2008</v>
@@ -762,22 +762,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10.01251990141416</v>
+        <v>9.944738096578352</v>
       </c>
       <c r="C12" t="n">
-        <v>9.884606327828703</v>
+        <v>9.955446779326929</v>
       </c>
       <c r="D12" t="n">
-        <v>21.24591571213848</v>
+        <v>1.994155829074569</v>
       </c>
       <c r="E12" t="n">
-        <v>1.352081796531384</v>
+        <v>-0.1204773828060981</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1782673482316987</v>
+        <v>0.9042744985259052</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>2009</v>
@@ -790,19 +790,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.88092943719562</v>
+        <v>5.796489503933924</v>
       </c>
       <c r="C13" t="n">
-        <v>5.89110239883107</v>
+        <v>5.842874110427214</v>
       </c>
       <c r="D13" t="n">
-        <v>1.261690494119749</v>
+        <v>5.748408457145337</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.08029349137356125</v>
+        <v>-0.3472914183134347</v>
       </c>
       <c r="F13" t="n">
-        <v>0.936111277566352</v>
+        <v>0.7289206274373221</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8941232088786617</v>
+        <v>0.8569433889038716</v>
       </c>
       <c r="C14" t="n">
-        <v>0.949989071809646</v>
+        <v>0.8106163152124527</v>
       </c>
       <c r="D14" t="n">
-        <v>13.60050726859344</v>
+        <v>20.56200810249328</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.8655309825479414</v>
+        <v>1.242258446059252</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3881945095287727</v>
+        <v>0.2161998651917395</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -842,23 +842,23 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.02816575964203389</v>
+        <v>-4.159683577438074</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01618092361170295</v>
+        <v>-4.359373052069835</v>
       </c>
       <c r="D15" t="n">
-        <v>59.1912889192968</v>
+        <v>20.01077250846795</v>
       </c>
       <c r="E15" t="n">
-        <v>3.766910560380623</v>
+        <v>1.208955420934803</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0002597619294976709</v>
+        <v>0.2287226000309382</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.309376160768184</v>
+        <v>2.158832244540103</v>
       </c>
       <c r="C16" t="n">
-        <v>2.420066594617967</v>
+        <v>2.298959209997159</v>
       </c>
       <c r="D16" t="n">
-        <v>8.529704693736033</v>
+        <v>11.18736457137918</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.5428270827413525</v>
+        <v>-0.6758872021966889</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5880388460890091</v>
+        <v>0.5002935070219086</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>2009</v>
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.11095056005873</v>
+        <v>10.10664326431772</v>
       </c>
       <c r="C17" t="n">
-        <v>10.06544336156333</v>
+        <v>10.06586110991063</v>
       </c>
       <c r="D17" t="n">
-        <v>8.345229376751675</v>
+        <v>7.808137970661496</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5310871454572467</v>
+        <v>0.4907338620342996</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5960948781490397</v>
+        <v>0.6243121683477533</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.908018674588855</v>
+        <v>5.888743636791447</v>
       </c>
       <c r="C18" t="n">
-        <v>5.907265978446604</v>
+        <v>5.792937961206031</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08939075227324814</v>
+        <v>9.901858143697098</v>
       </c>
       <c r="E18" t="n">
-        <v>0.005688792639700249</v>
+        <v>0.6223221344743468</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9954685810396141</v>
+        <v>0.53464033126795</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -958,22 +958,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8693140625827545</v>
+        <v>0.860177124439055</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8489856848282523</v>
+        <v>0.82069920632513</v>
       </c>
       <c r="D19" t="n">
-        <v>6.431237785566355</v>
+        <v>12.13338441343615</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4092814664637413</v>
+        <v>0.7625713857932582</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6828814886727602</v>
+        <v>0.4468712996905381</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>2010</v>
@@ -982,26 +982,26 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0271532080672045</v>
+        <v>-4.155354170038526</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01907334773020722</v>
+        <v>-4.166630380924821</v>
       </c>
       <c r="D20" t="n">
-        <v>35.57499677198165</v>
+        <v>1.041862843259531</v>
       </c>
       <c r="E20" t="n">
-        <v>2.263978931234199</v>
+        <v>0.06548006435130542</v>
       </c>
       <c r="F20" t="n">
-        <v>0.02536305067326974</v>
+        <v>0.9478832679118407</v>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>2010</v>
@@ -1014,22 +1014,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.283593376532411</v>
+        <v>2.232405669788315</v>
       </c>
       <c r="C21" t="n">
-        <v>2.38243941264437</v>
+        <v>2.396404415000481</v>
       </c>
       <c r="D21" t="n">
-        <v>7.039251296141972</v>
+        <v>12.09097168607363</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.4479752093380365</v>
+        <v>-0.7599057872118523</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6548312789013553</v>
+        <v>0.4485574965288163</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>2010</v>
@@ -1045,19 +1045,19 @@
         <v>10.23942163573567</v>
       </c>
       <c r="C22" t="n">
-        <v>10.17521816274095</v>
+        <v>10.28121836673852</v>
       </c>
       <c r="D22" t="n">
-        <v>11.38224999314063</v>
+        <v>7.181212332670568</v>
       </c>
       <c r="E22" t="n">
-        <v>0.7198766975152061</v>
+        <v>-0.4541797466505959</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4726722635167959</v>
+        <v>0.6503351907619035</v>
       </c>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
         <v>2011</v>
@@ -1073,16 +1073,16 @@
         <v>5.902029585362802</v>
       </c>
       <c r="C23" t="n">
-        <v>5.732676275330248</v>
+        <v>5.739600370862801</v>
       </c>
       <c r="D23" t="n">
-        <v>17.4894437803551</v>
+        <v>16.97606859693585</v>
       </c>
       <c r="E23" t="n">
-        <v>1.106129547107755</v>
+        <v>1.073660849631524</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2703531341286874</v>
+        <v>0.2846163140505338</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1101,19 +1101,19 @@
         <v>0.8133325961855089</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8941964044452699</v>
+        <v>0.8303285509948605</v>
       </c>
       <c r="D24" t="n">
-        <v>27.6712390550067</v>
+        <v>6.369362566271564</v>
       </c>
       <c r="E24" t="n">
-        <v>-1.750082821856529</v>
+        <v>-0.402833859056666</v>
       </c>
       <c r="F24" t="n">
-        <v>0.08225032235187749</v>
+        <v>0.687634710658704</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
         <v>2011</v>
@@ -1122,23 +1122,23 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0256839505611487</v>
+        <v>-4.174946423495506</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01814601413471573</v>
+        <v>-4.426698948148167</v>
       </c>
       <c r="D25" t="n">
-        <v>35.67819415318675</v>
+        <v>24.49731295263824</v>
       </c>
       <c r="E25" t="n">
-        <v>2.256487126515451</v>
+        <v>1.549346109685628</v>
       </c>
       <c r="F25" t="n">
-        <v>0.02607327728905738</v>
+        <v>0.123417816646718</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1157,16 +1157,16 @@
         <v>2.114114942899765</v>
       </c>
       <c r="C26" t="n">
-        <v>2.217092517472445</v>
+        <v>2.119274320347017</v>
       </c>
       <c r="D26" t="n">
-        <v>8.389704122245792</v>
+        <v>0.423493328247691</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.5306114784240086</v>
+        <v>-0.02678406982296055</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5965311560809884</v>
+        <v>0.9786699787735358</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1185,19 +1185,19 @@
         <v>10.3330699093908</v>
       </c>
       <c r="C27" t="n">
-        <v>10.38005510895234</v>
+        <v>10.39372442806099</v>
       </c>
       <c r="D27" t="n">
-        <v>8.325008695991384</v>
+        <v>10.89484661989024</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.5395222267071071</v>
+        <v>-0.7060667589243397</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5902616251770103</v>
+        <v>0.4811473601913111</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
         <v>2012</v>
@@ -1213,19 +1213,19 @@
         <v>5.947867890617655</v>
       </c>
       <c r="C28" t="n">
-        <v>5.87986006304322</v>
+        <v>5.831988881966329</v>
       </c>
       <c r="D28" t="n">
-        <v>6.913000865507928</v>
+        <v>11.82134434152247</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4480136605722599</v>
+        <v>0.7661106738399815</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6547296894119602</v>
+        <v>0.4447017110189228</v>
       </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>2012</v>
@@ -1241,16 +1241,16 @@
         <v>0.8408123037517883</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8362266517005471</v>
+        <v>0.8307227554680235</v>
       </c>
       <c r="D29" t="n">
-        <v>1.603734091634853</v>
+        <v>3.312590331547823</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1039338479708216</v>
+        <v>0.2146803897881437</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9173546600105469</v>
+        <v>0.8303090506243311</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1262,26 +1262,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02528113577680486</v>
+        <v>-4.177973982144462</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01872028265090898</v>
+        <v>-4.192713194709146</v>
       </c>
       <c r="D30" t="n">
-        <v>32.63762264587828</v>
+        <v>1.568226673438571</v>
       </c>
       <c r="E30" t="n">
-        <v>2.115159693804214</v>
+        <v>0.1016327042688212</v>
       </c>
       <c r="F30" t="n">
-        <v>0.03675529456226291</v>
+        <v>0.9191888885993031</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
         <v>2012</v>
@@ -1297,16 +1297,16 @@
         <v>2.200553102795348</v>
       </c>
       <c r="C31" t="n">
-        <v>2.145773824283834</v>
+        <v>2.163361332334392</v>
       </c>
       <c r="D31" t="n">
-        <v>4.87616942257653</v>
+        <v>3.246519542323875</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3160118962922367</v>
+        <v>0.210398513261148</v>
       </c>
       <c r="F31" t="n">
-        <v>0.7524170860768922</v>
+        <v>0.8336359939302548</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -1325,16 +1325,16 @@
         <v>10.43251584686971</v>
       </c>
       <c r="C32" t="n">
-        <v>10.47735058858488</v>
+        <v>10.43743124418211</v>
       </c>
       <c r="D32" t="n">
-        <v>8.214669331186252</v>
+        <v>0.9613599798445172</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.5195413062336121</v>
+        <v>-0.0608017437528448</v>
       </c>
       <c r="F32" t="n">
-        <v>0.604140179086649</v>
+        <v>0.9515945828375385</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1353,16 +1353,16 @@
         <v>5.958671399571555</v>
       </c>
       <c r="C33" t="n">
-        <v>5.767407368497618</v>
+        <v>5.786809720891723</v>
       </c>
       <c r="D33" t="n">
-        <v>18.70529265515308</v>
+        <v>17.72760261446441</v>
       </c>
       <c r="E33" t="n">
-        <v>1.183026581806045</v>
+        <v>1.121192034321267</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2386454452030831</v>
+        <v>0.2639271815980185</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1381,19 +1381,19 @@
         <v>0.8475464717182144</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8272590225516019</v>
+        <v>0.8785000517825547</v>
       </c>
       <c r="D34" t="n">
-        <v>8.024322784781265</v>
+        <v>10.98974525962402</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5075027336058783</v>
+        <v>-0.6950525185090075</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6125098769573742</v>
+        <v>0.4880854169020128</v>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>2013</v>
@@ -1402,23 +1402,23 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.02568824640355542</v>
+        <v>-4.144654605692573</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01668430337418548</v>
+        <v>-4.243482036992442</v>
       </c>
       <c r="D35" t="n">
-        <v>44.2712010660398</v>
+        <v>10.13731348163677</v>
       </c>
       <c r="E35" t="n">
-        <v>2.799956602399204</v>
+        <v>0.6411399991420739</v>
       </c>
       <c r="F35" t="n">
-        <v>0.006046164553475626</v>
+        <v>0.5224416818255502</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -1437,16 +1437,16 @@
         <v>2.299863928968326</v>
       </c>
       <c r="C36" t="n">
-        <v>2.396732110093257</v>
+        <v>2.423903792803384</v>
       </c>
       <c r="D36" t="n">
-        <v>7.36480609150935</v>
+        <v>9.144787586994925</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.4657912354930402</v>
+        <v>-0.5783671498667829</v>
       </c>
       <c r="F36" t="n">
-        <v>0.642118180178531</v>
+        <v>0.56400811029015</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1465,16 +1465,16 @@
         <v>10.48241045137295</v>
       </c>
       <c r="C37" t="n">
-        <v>10.52668535611424</v>
+        <v>10.4594990597563</v>
       </c>
       <c r="D37" t="n">
-        <v>8.34072298851739</v>
+        <v>4.219296377798996</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.5373134921816195</v>
+        <v>0.2718091554443798</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5917974715913383</v>
+        <v>0.7861236391961248</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1493,19 +1493,19 @@
         <v>5.959495247718891</v>
       </c>
       <c r="C38" t="n">
-        <v>5.795072823250485</v>
+        <v>5.889417395384815</v>
       </c>
       <c r="D38" t="n">
-        <v>16.81836746219149</v>
+        <v>7.810887972192197</v>
       </c>
       <c r="E38" t="n">
-        <v>1.083447534026083</v>
+        <v>0.5031812588855704</v>
       </c>
       <c r="F38" t="n">
-        <v>0.2802105430154713</v>
+        <v>0.6155175818822256</v>
       </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
         <v>2014</v>
@@ -1521,16 +1521,16 @@
         <v>0.9122236200008085</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9722295470196882</v>
+        <v>0.9557828746555302</v>
       </c>
       <c r="D39" t="n">
-        <v>14.17354146960843</v>
+        <v>11.59371261023261</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.9130665380088383</v>
+        <v>-0.7468726893975748</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3625562356184717</v>
+        <v>0.4562404572958972</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1542,26 +1542,26 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02293646088886293</v>
+        <v>-4.246024440364211</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01726125052109377</v>
+        <v>-4.272389160813397</v>
       </c>
       <c r="D40" t="n">
-        <v>30.07011053217019</v>
+        <v>2.611479572594593</v>
       </c>
       <c r="E40" t="n">
-        <v>1.937131364100089</v>
+        <v>0.1682328031806734</v>
       </c>
       <c r="F40" t="n">
-        <v>0.05506757259805677</v>
+        <v>0.8666127629070691</v>
       </c>
       <c r="G40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
         <v>2014</v>
@@ -1577,19 +1577,19 @@
         <v>2.399537896289476</v>
       </c>
       <c r="C41" t="n">
-        <v>2.42821286832377</v>
+        <v>2.615481501607051</v>
       </c>
       <c r="D41" t="n">
-        <v>2.041455312201931</v>
+        <v>14.62089600582008</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.1315115589430357</v>
+        <v>-0.9418853380608347</v>
       </c>
       <c r="F41" t="n">
-        <v>0.8955636663602962</v>
+        <v>0.3479791282229356</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>2014</v>
@@ -1602,19 +1602,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.52652732126093</v>
+        <v>10.53467826582806</v>
       </c>
       <c r="C42" t="n">
-        <v>10.4844310223596</v>
+        <v>10.52785832041014</v>
       </c>
       <c r="D42" t="n">
-        <v>8.652892284127326</v>
+        <v>1.454023263255139</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5438258473802117</v>
+        <v>0.09253347385056314</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5873380603714987</v>
+        <v>0.9263902541305575</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1630,19 +1630,19 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5.983023124981512</v>
+        <v>6.018570300320664</v>
       </c>
       <c r="C43" t="n">
-        <v>5.890745399699154</v>
+        <v>5.943542266852779</v>
       </c>
       <c r="D43" t="n">
-        <v>9.669867400820893</v>
+        <v>9.145236844479376</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6077417423711831</v>
+        <v>0.5819993089459587</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5442428583276481</v>
+        <v>0.5615012445702342</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -1658,19 +1658,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9545176410858773</v>
+        <v>0.9953619466772416</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9414163852693048</v>
+        <v>0.9614970396226129</v>
       </c>
       <c r="D44" t="n">
-        <v>4.525713734975136</v>
+        <v>8.172857480881108</v>
       </c>
       <c r="E44" t="n">
-        <v>0.2844366977083359</v>
+        <v>0.5201174651762012</v>
       </c>
       <c r="F44" t="n">
-        <v>0.7764538809729156</v>
+        <v>0.603707629513682</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -1682,26 +1682,26 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.01889017056373976</v>
+        <v>-4.557257529927539</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01382031413892792</v>
+        <v>-4.668177890201437</v>
       </c>
       <c r="D45" t="n">
-        <v>31.19701692472276</v>
+        <v>9.391931559907597</v>
       </c>
       <c r="E45" t="n">
-        <v>1.960702110662321</v>
+        <v>0.5976988645005551</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0519945286464719</v>
+        <v>0.5509681665630712</v>
       </c>
       <c r="G45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
         <v>2015</v>
@@ -1714,22 +1714,22 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.496784392767126</v>
+        <v>2.574653801191209</v>
       </c>
       <c r="C46" t="n">
-        <v>2.707259782640725</v>
+        <v>2.588045373273864</v>
       </c>
       <c r="D46" t="n">
-        <v>15.71282133956197</v>
+        <v>1.032808678889809</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.9875355082595899</v>
+        <v>-0.06572754184601733</v>
       </c>
       <c r="F46" t="n">
-        <v>0.3252077368722279</v>
+        <v>0.9476824700282682</v>
       </c>
       <c r="G46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
         <v>2015</v>
@@ -1742,19 +1742,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.59040599580133</v>
+        <v>10.59668476642354</v>
       </c>
       <c r="C47" t="n">
-        <v>10.59344859437135</v>
+        <v>10.60191466941132</v>
       </c>
       <c r="D47" t="n">
-        <v>0.5825527468612985</v>
+        <v>1.01972406641728</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.03470958578272776</v>
+        <v>-0.05989522720656087</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9723628865051106</v>
+        <v>0.9523310973343649</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -1770,19 +1770,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6.092075162246972</v>
+        <v>6.085096833259739</v>
       </c>
       <c r="C48" t="n">
-        <v>6.082523482630344</v>
+        <v>6.127050493752438</v>
       </c>
       <c r="D48" t="n">
-        <v>1.071081772891645</v>
+        <v>5.228246171010966</v>
       </c>
       <c r="E48" t="n">
-        <v>0.06381706184856456</v>
+        <v>-0.3070899301266379</v>
       </c>
       <c r="F48" t="n">
-        <v>0.9492079901693098</v>
+        <v>0.759252117318842</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1798,22 +1798,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1.025071902164961</v>
+        <v>0.9771317506091897</v>
       </c>
       <c r="C49" t="n">
-        <v>1.019416744764289</v>
+        <v>0.9396668346811998</v>
       </c>
       <c r="D49" t="n">
-        <v>1.428224825319543</v>
+        <v>14.41470136896961</v>
       </c>
       <c r="E49" t="n">
-        <v>0.08509631506939409</v>
+        <v>0.8466719988697994</v>
       </c>
       <c r="F49" t="n">
-        <v>0.9323189935250483</v>
+        <v>0.3986654379458929</v>
       </c>
       <c r="G49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
         <v>2016</v>
@@ -1822,26 +1822,26 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.01728606665297535</v>
+        <v>-4.597813058997881</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01993632363240273</v>
+        <v>-4.515118120630742</v>
       </c>
       <c r="D50" t="n">
-        <v>16.71055321733946</v>
+        <v>7.10579124036679</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.9956461170239385</v>
+        <v>-0.4173707327703671</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3211433496980751</v>
+        <v>0.6771145869480375</v>
       </c>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="n">
         <v>2016</v>
@@ -1854,19 +1854,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.725645929551326</v>
+        <v>2.657614703827844</v>
       </c>
       <c r="C51" t="n">
-        <v>2.714799200087747</v>
+        <v>2.678686335073336</v>
       </c>
       <c r="D51" t="n">
-        <v>0.8687239428683954</v>
+        <v>1.709829883302616</v>
       </c>
       <c r="E51" t="n">
-        <v>0.05176020262364203</v>
+        <v>-0.1004297659706996</v>
       </c>
       <c r="F51" t="n">
-        <v>0.9587935463032669</v>
+        <v>0.9201546873289521</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1885,19 +1885,19 @@
         <v>10.73836324580539</v>
       </c>
       <c r="C52" t="n">
-        <v>10.70165509723754</v>
+        <v>10.65006685539413</v>
       </c>
       <c r="D52" t="n">
-        <v>7.554361576033807</v>
+        <v>17.55392155718831</v>
       </c>
       <c r="E52" t="n">
-        <v>0.3700866238754035</v>
+        <v>0.8599630159990657</v>
       </c>
       <c r="F52" t="n">
-        <v>0.7121929555206569</v>
+        <v>0.3921656828114156</v>
       </c>
       <c r="G52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
         <v>2017</v>
@@ -1913,19 +1913,19 @@
         <v>5.989743211503313</v>
       </c>
       <c r="C53" t="n">
-        <v>5.763949609822437</v>
+        <v>5.955417152935073</v>
       </c>
       <c r="D53" t="n">
-        <v>23.08802269011959</v>
+        <v>4.000737185714197</v>
       </c>
       <c r="E53" t="n">
-        <v>1.131077495211865</v>
+        <v>0.1959952939995633</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2609359488249487</v>
+        <v>0.8451204593155049</v>
       </c>
       <c r="G53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
         <v>2017</v>
@@ -1941,16 +1941,16 @@
         <v>1.049421545455431</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9446680319675788</v>
+        <v>0.9745060217859275</v>
       </c>
       <c r="D54" t="n">
-        <v>21.0898680388664</v>
+        <v>14.98385079473149</v>
       </c>
       <c r="E54" t="n">
-        <v>1.03318830875708</v>
+        <v>0.734055776581767</v>
       </c>
       <c r="F54" t="n">
-        <v>0.3055172716367514</v>
+        <v>0.4656161820485321</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1962,23 +1962,23 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.02113660227811425</v>
+        <v>-4.33983385800687</v>
       </c>
       <c r="C55" t="n">
-        <v>0.01248137810771285</v>
+        <v>-4.437909592468015</v>
       </c>
       <c r="D55" t="n">
-        <v>63.91977481210395</v>
+        <v>10.31542385680363</v>
       </c>
       <c r="E55" t="n">
-        <v>3.131416655265184</v>
+        <v>0.5053504985940278</v>
       </c>
       <c r="F55" t="n">
-        <v>0.002584228450654275</v>
+        <v>0.614785342937795</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -1997,16 +1997,16 @@
         <v>2.832824404287503</v>
       </c>
       <c r="C56" t="n">
-        <v>2.817896588874907</v>
+        <v>2.896001604570449</v>
       </c>
       <c r="D56" t="n">
-        <v>1.122481639184733</v>
+        <v>4.779955478132232</v>
       </c>
       <c r="E56" t="n">
-        <v>0.05499014523290904</v>
+        <v>-0.2341690382929033</v>
       </c>
       <c r="F56" t="n">
-        <v>0.9562665025454542</v>
+        <v>0.8153764491643476</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.74488675502338</v>
+        <v>10.73209550212109</v>
       </c>
       <c r="C57" t="n">
-        <v>10.74948372494864</v>
+        <v>10.65854977980649</v>
       </c>
       <c r="D57" t="n">
-        <v>0.8848330242563269</v>
+        <v>14.17974893276519</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.05044324347866068</v>
+        <v>0.7831022304773366</v>
       </c>
       <c r="F57" t="n">
-        <v>0.95985051710256</v>
+        <v>0.4351519722747588</v>
       </c>
       <c r="G57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
         <v>2018</v>
@@ -2050,22 +2050,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6.133565251852714</v>
+        <v>6.101464207182762</v>
       </c>
       <c r="C58" t="n">
-        <v>5.91170478041134</v>
+        <v>6.15636456769754</v>
       </c>
       <c r="D58" t="n">
-        <v>21.55926271333818</v>
+        <v>6.096887235950424</v>
       </c>
       <c r="E58" t="n">
-        <v>1.229067076450218</v>
+        <v>-0.336711603010767</v>
       </c>
       <c r="F58" t="n">
-        <v>0.2213539759428255</v>
+        <v>0.7369285138841576</v>
       </c>
       <c r="G58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
         <v>2018</v>
@@ -2078,19 +2078,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.119738877635338</v>
+        <v>1.193539584552961</v>
       </c>
       <c r="C59" t="n">
-        <v>1.209895037495459</v>
+        <v>1.106109955652392</v>
       </c>
       <c r="D59" t="n">
-        <v>19.00882571609166</v>
+        <v>15.37286771840096</v>
       </c>
       <c r="E59" t="n">
-        <v>-1.083669797074011</v>
+        <v>0.8489943690960122</v>
       </c>
       <c r="F59" t="n">
-        <v>0.2806163956604502</v>
+        <v>0.3982814956537148</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2102,26 +2102,26 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.01579379514489403</v>
+        <v>-4.718514302826229</v>
       </c>
       <c r="C60" t="n">
-        <v>0.01693373312297062</v>
+        <v>-4.906488624161423</v>
       </c>
       <c r="D60" t="n">
-        <v>7.434345543653027</v>
+        <v>12.09481487939683</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.4238229045284236</v>
+        <v>0.6679579838949309</v>
       </c>
       <c r="F60" t="n">
-        <v>0.6724064701834606</v>
+        <v>0.5056201038525776</v>
       </c>
       <c r="G60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
         <v>2018</v>
@@ -2134,22 +2134,22 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.874527139398365</v>
+        <v>2.854853126466251</v>
       </c>
       <c r="C61" t="n">
-        <v>3.065139288798557</v>
+        <v>2.79398611983693</v>
       </c>
       <c r="D61" t="n">
-        <v>13.96271447634037</v>
+        <v>4.511455880813097</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.7959971956799632</v>
+        <v>0.249153294583466</v>
       </c>
       <c r="F61" t="n">
-        <v>0.4275516574453077</v>
+        <v>0.803669109636034</v>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
         <v>2018</v>
@@ -2165,16 +2165,16 @@
         <v>10.79839271553016</v>
       </c>
       <c r="C62" t="n">
-        <v>10.86998828753738</v>
+        <v>10.88636647851982</v>
       </c>
       <c r="D62" t="n">
-        <v>13.67242454881587</v>
+        <v>17.51873359267034</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.7362825950848504</v>
+        <v>-0.9434126760881332</v>
       </c>
       <c r="F62" t="n">
-        <v>0.4631303258279708</v>
+        <v>0.3474975411935338</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2193,19 +2193,19 @@
         <v>6.100189458613614</v>
       </c>
       <c r="C63" t="n">
-        <v>6.004448482299269</v>
+        <v>5.928017145247848</v>
       </c>
       <c r="D63" t="n">
-        <v>8.992933867035303</v>
+        <v>15.6815636891267</v>
       </c>
       <c r="E63" t="n">
-        <v>0.4842843097364651</v>
+        <v>0.8444780489952342</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6291147113912066</v>
+        <v>0.4001718983939448</v>
       </c>
       <c r="G63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
         <v>2019</v>
@@ -2221,16 +2221,16 @@
         <v>1.185227990036963</v>
       </c>
       <c r="C64" t="n">
-        <v>1.130871517485383</v>
+        <v>1.136780430519192</v>
       </c>
       <c r="D64" t="n">
-        <v>15.99520569995711</v>
+        <v>15.34846461189549</v>
       </c>
       <c r="E64" t="n">
-        <v>0.8613681881828623</v>
+        <v>0.8265401147152894</v>
       </c>
       <c r="F64" t="n">
-        <v>0.3908643339052892</v>
+        <v>0.4103631493447627</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -2242,23 +2242,23 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>fdi_openness</t>
+          <t>ln_fdi_openness</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.01585353670661224</v>
+        <v>-4.726792153276239</v>
       </c>
       <c r="C65" t="n">
-        <v>0.01173552849476199</v>
+        <v>-5.176148458535523</v>
       </c>
       <c r="D65" t="n">
-        <v>29.00057234465861</v>
+        <v>31.33677741854512</v>
       </c>
       <c r="E65" t="n">
-        <v>1.561728615772137</v>
+        <v>1.687537109233564</v>
       </c>
       <c r="F65" t="n">
-        <v>0.1213041392925123</v>
+        <v>0.0944914371721062</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2277,19 +2277,19 @@
         <v>2.89832919103753</v>
       </c>
       <c r="C66" t="n">
-        <v>2.781509390211292</v>
+        <v>2.755727279122699</v>
       </c>
       <c r="D66" t="n">
-        <v>9.998394978642592</v>
+        <v>12.69756988854078</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5384300476681643</v>
+        <v>0.683785064999006</v>
       </c>
       <c r="F66" t="n">
-        <v>0.5913299647196826</v>
+        <v>0.4955084437672063</v>
       </c>
       <c r="G66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>2019</v>

</xml_diff>

<commit_message>
Tighten PSM caliper from 0.05 to 0.02 for stricter matching
Changes:
- Reduced caliper from 0.05 to 0.02 for more stringent matching criteria
- Higher quality matches with smaller propensity score differences
- Trade-off: lower match rate (66-93% vs 89-96%) but better balance

Results with caliper=0.02:
- Total matched samples: 1,732 (vs 1,886 with caliper=0.05)
- Average standardized bias:
  * ln_pgdp: 9.11% (GOOD)
  * financial_development: 8.41% (GOOD)
  * ln_fdi_openness: 13.00%
  * ln_pop_density: 13.63%
  * industrial_advanced: 17.27%
- 2/5 variables pass <10% threshold

Stricter caliper prioritizes match quality over quantity
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -482,22 +482,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.866885858537243</v>
+        <v>9.831061709726443</v>
       </c>
       <c r="C2" t="n">
-        <v>9.796858244112498</v>
+        <v>9.793361061724081</v>
       </c>
       <c r="D2" t="n">
-        <v>12.35099877627559</v>
+        <v>6.506870464907174</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7358956829870943</v>
+        <v>0.3680841784030661</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4630398185859812</v>
+        <v>0.713432102243335</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>2007</v>
@@ -510,19 +510,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.936590613538837</v>
+        <v>5.896404323736572</v>
       </c>
       <c r="C3" t="n">
-        <v>5.544140453629207</v>
+        <v>5.53742500803248</v>
       </c>
       <c r="D3" t="n">
-        <v>43.45956242412928</v>
+        <v>38.63978847710614</v>
       </c>
       <c r="E3" t="n">
-        <v>2.589402278450299</v>
+        <v>2.185796516462045</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01063014453517161</v>
+        <v>0.03067944459355844</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.867083535175366</v>
+        <v>0.8343211364355647</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8771512619902208</v>
+        <v>0.8611218509132418</v>
       </c>
       <c r="D4" t="n">
-        <v>2.939690870118161</v>
+        <v>9.554165115143155</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1751522981924275</v>
+        <v>-0.5404651953194941</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8612410819124753</v>
+        <v>0.5898306191154187</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-3.95563786284638</v>
+        <v>-4.007612164593573</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.311539890514882</v>
+        <v>-4.341957496718453</v>
       </c>
       <c r="D5" t="n">
-        <v>32.34627326450113</v>
+        <v>29.47762433334325</v>
       </c>
       <c r="E5" t="n">
-        <v>1.927251656909735</v>
+        <v>1.667506244750128</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05636921911241014</v>
+        <v>0.09838273182892644</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -594,19 +594,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.97459045550319</v>
+        <v>1.832194796766036</v>
       </c>
       <c r="C6" t="n">
-        <v>2.030481192103107</v>
+        <v>1.880197441810711</v>
       </c>
       <c r="D6" t="n">
-        <v>5.51500034149419</v>
+        <v>5.383435601501279</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3285940689083077</v>
+        <v>-0.3045331055922108</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7429585260453673</v>
+        <v>0.761232559759102</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -622,19 +622,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.941805817671584</v>
+        <v>9.893568607345104</v>
       </c>
       <c r="C7" t="n">
-        <v>9.825528099581071</v>
+        <v>9.829904583490093</v>
       </c>
       <c r="D7" t="n">
-        <v>21.78357253987299</v>
+        <v>12.05489296821627</v>
       </c>
       <c r="E7" t="n">
-        <v>1.342829595994835</v>
+        <v>0.7182531433184142</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1814004727385762</v>
+        <v>0.4738078940923257</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.91997438393599</v>
+        <v>5.830136567026361</v>
       </c>
       <c r="C8" t="n">
-        <v>5.847710969680237</v>
+        <v>5.850878607499658</v>
       </c>
       <c r="D8" t="n">
-        <v>8.944868383876276</v>
+        <v>2.621587344944157</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5513987192028139</v>
+        <v>-0.156199093260679</v>
       </c>
       <c r="F8" t="n">
-        <v>0.582239286441933</v>
+        <v>0.8761089170022287</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -678,19 +678,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8232495113715774</v>
+        <v>0.8160652605894007</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7718025735245637</v>
+        <v>0.7640367752147221</v>
       </c>
       <c r="D9" t="n">
-        <v>22.51015062757064</v>
+        <v>23.12300236666415</v>
       </c>
       <c r="E9" t="n">
-        <v>1.387618877375374</v>
+        <v>1.377711869910789</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1673124880423143</v>
+        <v>0.1704953540543297</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -706,19 +706,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4.009049540374143</v>
+        <v>-4.079403587289681</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.070772577035275</v>
+        <v>-4.047832342663729</v>
       </c>
       <c r="D10" t="n">
-        <v>6.329428013209025</v>
+        <v>3.199347790857023</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3901721467540982</v>
+        <v>-0.1906231447604385</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6970921886852728</v>
+        <v>0.8491577031926544</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -734,22 +734,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.989491080568654</v>
+        <v>1.922261466366433</v>
       </c>
       <c r="C11" t="n">
-        <v>2.166964103316953</v>
+        <v>2.025413593517064</v>
       </c>
       <c r="D11" t="n">
-        <v>15.98590910217347</v>
+        <v>9.930846619091945</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.985437619196273</v>
+        <v>-0.5916984761940419</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3261027945507792</v>
+        <v>0.5550584514864572</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>2008</v>
@@ -762,19 +762,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.944738096578352</v>
+        <v>9.902065307870203</v>
       </c>
       <c r="C12" t="n">
-        <v>9.955446779326929</v>
+        <v>9.939595678788933</v>
       </c>
       <c r="D12" t="n">
-        <v>1.994155829074569</v>
+        <v>6.918364337051003</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1204773828060981</v>
+        <v>-0.4004292859989141</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9042744985259052</v>
+        <v>0.6894900908258059</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -790,22 +790,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.796489503933924</v>
+        <v>5.729139006306387</v>
       </c>
       <c r="C13" t="n">
-        <v>5.842874110427214</v>
+        <v>5.838702428465379</v>
       </c>
       <c r="D13" t="n">
-        <v>5.748408457145337</v>
+        <v>13.53612219654284</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.3472914183134347</v>
+        <v>-0.7834597142170922</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7289206274373221</v>
+        <v>0.4348373488259066</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>2009</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8569433889038716</v>
+        <v>0.8366142252361952</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8106163152124527</v>
+        <v>0.7900212143625021</v>
       </c>
       <c r="D14" t="n">
-        <v>20.56200810249328</v>
+        <v>21.47404143716593</v>
       </c>
       <c r="E14" t="n">
-        <v>1.242258446059252</v>
+        <v>1.242900006601959</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2161998651917395</v>
+        <v>0.2161509537101326</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -846,19 +846,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-4.159683577438074</v>
+        <v>-4.208259657959464</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.359373052069835</v>
+        <v>-4.311127024150943</v>
       </c>
       <c r="D15" t="n">
-        <v>20.01077250846795</v>
+        <v>10.28803810182849</v>
       </c>
       <c r="E15" t="n">
-        <v>1.208955420934803</v>
+        <v>0.5954632555822909</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2287226000309382</v>
+        <v>0.5525822864267149</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.158832244540103</v>
+        <v>2.003679992214923</v>
       </c>
       <c r="C16" t="n">
-        <v>2.298959209997159</v>
+        <v>2.04696325794343</v>
       </c>
       <c r="D16" t="n">
-        <v>11.18736457137918</v>
+        <v>4.225096485968105</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.6758872021966889</v>
+        <v>-0.2445451391005945</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5002935070219086</v>
+        <v>0.8072104774265709</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>2009</v>
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.10664326431772</v>
+        <v>10.07142485723458</v>
       </c>
       <c r="C17" t="n">
-        <v>10.06586110991063</v>
+        <v>10.04600262706136</v>
       </c>
       <c r="D17" t="n">
-        <v>7.808137970661496</v>
+        <v>4.897239080105492</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4907338620342996</v>
+        <v>0.2978874237837781</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6243121683477533</v>
+        <v>0.7662164051941887</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.888743636791447</v>
+        <v>5.825947485097656</v>
       </c>
       <c r="C18" t="n">
-        <v>5.792937961206031</v>
+        <v>5.740545715147354</v>
       </c>
       <c r="D18" t="n">
-        <v>9.901858143697098</v>
+        <v>8.907592211278009</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6223221344743468</v>
+        <v>0.5418276813793813</v>
       </c>
       <c r="F18" t="n">
-        <v>0.53464033126795</v>
+        <v>0.5887683735682281</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -958,22 +958,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.860177124439055</v>
+        <v>0.8181311529903835</v>
       </c>
       <c r="C19" t="n">
-        <v>0.82069920632513</v>
+        <v>0.8014471342338714</v>
       </c>
       <c r="D19" t="n">
-        <v>12.13338441343615</v>
+        <v>5.951004605254284</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7625713857932582</v>
+        <v>0.3619854783047291</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4468712996905381</v>
+        <v>0.7179600716403638</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
         <v>2010</v>
@@ -986,19 +986,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-4.155354170038526</v>
+        <v>-4.244840813804466</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.166630380924821</v>
+        <v>-4.159135045303332</v>
       </c>
       <c r="D20" t="n">
-        <v>1.041862843259531</v>
+        <v>7.946893495736044</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06548006435130542</v>
+        <v>-0.4833906598813384</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9478832679118407</v>
+        <v>0.6295934618793155</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1014,22 +1014,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.232405669788315</v>
+        <v>2.064302915813227</v>
       </c>
       <c r="C21" t="n">
-        <v>2.396404415000481</v>
+        <v>2.158606665564263</v>
       </c>
       <c r="D21" t="n">
-        <v>12.09097168607363</v>
+        <v>8.800969493744422</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.7599057872118523</v>
+        <v>-0.5353420746684626</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4485574965288163</v>
+        <v>0.5932821427275843</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>2010</v>
@@ -1042,19 +1042,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.23942163573567</v>
+        <v>10.19344865041129</v>
       </c>
       <c r="C22" t="n">
-        <v>10.28121836673852</v>
+        <v>10.24774486579877</v>
       </c>
       <c r="D22" t="n">
-        <v>7.181212332670568</v>
+        <v>9.387809457322378</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.4541797466505959</v>
+        <v>-0.567166666320861</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6503351907619035</v>
+        <v>0.571506889983673</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -1070,19 +1070,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.902029585362802</v>
+        <v>5.79625618531315</v>
       </c>
       <c r="C23" t="n">
-        <v>5.739600370862801</v>
+        <v>5.638520377735698</v>
       </c>
       <c r="D23" t="n">
-        <v>16.97606859693585</v>
+        <v>17.18531091890465</v>
       </c>
       <c r="E23" t="n">
-        <v>1.073660849631524</v>
+        <v>1.038254509518208</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2846163140505338</v>
+        <v>0.3008935663962301</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1098,19 +1098,19 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.8133325961855089</v>
+        <v>0.7874197663375814</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8303285509948605</v>
+        <v>0.8132273906556085</v>
       </c>
       <c r="D24" t="n">
-        <v>6.369362566271564</v>
+        <v>9.824508954401342</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.402833859056666</v>
+        <v>-0.5935499668201146</v>
       </c>
       <c r="F24" t="n">
-        <v>0.687634710658704</v>
+        <v>0.5538062382025568</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -1126,19 +1126,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-4.174946423495506</v>
+        <v>-4.243012104507941</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.426698948148167</v>
+        <v>-4.500456033115954</v>
       </c>
       <c r="D25" t="n">
-        <v>24.49731295263824</v>
+        <v>24.64340600912377</v>
       </c>
       <c r="E25" t="n">
-        <v>1.549346109685628</v>
+        <v>1.488837038770996</v>
       </c>
       <c r="F25" t="n">
-        <v>0.123417816646718</v>
+        <v>0.1388634852498884</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1154,19 +1154,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.114114942899765</v>
+        <v>1.90400699196487</v>
       </c>
       <c r="C26" t="n">
-        <v>2.119274320347017</v>
+        <v>1.87656195358794</v>
       </c>
       <c r="D26" t="n">
-        <v>0.423493328247691</v>
+        <v>3.064349788811842</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.02678406982296055</v>
+        <v>0.1851333968869415</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9786699787735358</v>
+        <v>0.853431084434499</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1182,19 +1182,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.3330699093908</v>
+        <v>10.27469335276085</v>
       </c>
       <c r="C27" t="n">
-        <v>10.39372442806099</v>
+        <v>10.35428343623804</v>
       </c>
       <c r="D27" t="n">
-        <v>10.89484661989024</v>
+        <v>14.62904042815387</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.7060667589243397</v>
+        <v>-0.9017946166531096</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4811473601913111</v>
+        <v>0.368639704822749</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -1210,19 +1210,19 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.947867890617655</v>
+        <v>5.822736552934555</v>
       </c>
       <c r="C28" t="n">
-        <v>5.831988881966329</v>
+        <v>5.721423620801668</v>
       </c>
       <c r="D28" t="n">
-        <v>11.82134434152247</v>
+        <v>10.85293329125018</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7661106738399815</v>
+        <v>0.669019739538708</v>
       </c>
       <c r="F28" t="n">
-        <v>0.4447017110189228</v>
+        <v>0.5045249311364384</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -1238,19 +1238,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8408123037517883</v>
+        <v>0.8067802742767602</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8307227554680235</v>
+        <v>0.8103035318118849</v>
       </c>
       <c r="D29" t="n">
-        <v>3.312590331547823</v>
+        <v>1.16656591066682</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2146803897881437</v>
+        <v>-0.07191195235100803</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8303090506243311</v>
+        <v>0.9427843225540449</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.177973982144462</v>
+        <v>-4.263727066615536</v>
       </c>
       <c r="C30" t="n">
-        <v>-4.192713194709146</v>
+        <v>-4.254713189811389</v>
       </c>
       <c r="D30" t="n">
-        <v>1.568226673438571</v>
+        <v>0.9473789159710863</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1016327042688212</v>
+        <v>-0.05840035855729732</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9191888885993031</v>
+        <v>0.9535189736287069</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1294,22 +1294,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.200553102795348</v>
+        <v>2.006216308500471</v>
       </c>
       <c r="C31" t="n">
-        <v>2.163361332334392</v>
+        <v>1.91967421242199</v>
       </c>
       <c r="D31" t="n">
-        <v>3.246519542323875</v>
+        <v>10.6512517289047</v>
       </c>
       <c r="E31" t="n">
-        <v>0.210398513261148</v>
+        <v>0.6565872530680763</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8336359939302548</v>
+        <v>0.5124724142717166</v>
       </c>
       <c r="G31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>2012</v>
@@ -1322,19 +1322,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10.43251584686971</v>
+        <v>10.38612977746011</v>
       </c>
       <c r="C32" t="n">
-        <v>10.43743124418211</v>
+        <v>10.41017709762223</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9613599798445172</v>
+        <v>4.875810925575722</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.0608017437528448</v>
+        <v>-0.2985812212486971</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9515945828375385</v>
+        <v>0.7656831541579039</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1350,19 +1350,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5.958671399571555</v>
+        <v>5.905446086039507</v>
       </c>
       <c r="C33" t="n">
-        <v>5.786809720891723</v>
+        <v>5.761157413124963</v>
       </c>
       <c r="D33" t="n">
-        <v>17.72760261446441</v>
+        <v>14.81203018340939</v>
       </c>
       <c r="E33" t="n">
-        <v>1.121192034321267</v>
+        <v>0.9070479001014033</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2639271815980185</v>
+        <v>0.3658743561347727</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1378,22 +1378,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.8475464717182144</v>
+        <v>0.8398055093164044</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8785000517825547</v>
+        <v>0.8679561117347987</v>
       </c>
       <c r="D34" t="n">
-        <v>10.98974525962402</v>
+        <v>9.942134993185444</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.6950525185090075</v>
+        <v>-0.6088289421793361</v>
       </c>
       <c r="F34" t="n">
-        <v>0.4880854169020128</v>
+        <v>0.5436163477710321</v>
       </c>
       <c r="G34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
         <v>2013</v>
@@ -1406,22 +1406,22 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-4.144654605692573</v>
+        <v>-4.177897145525887</v>
       </c>
       <c r="C35" t="n">
-        <v>-4.243482036992442</v>
+        <v>-4.234198662733117</v>
       </c>
       <c r="D35" t="n">
-        <v>10.13731348163677</v>
+        <v>5.730914506575491</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6411399991420739</v>
+        <v>0.3509454075155996</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5224416818255502</v>
+        <v>0.7261817636988828</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
         <v>2013</v>
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.299863928968326</v>
+        <v>2.248064065886551</v>
       </c>
       <c r="C36" t="n">
-        <v>2.423903792803384</v>
+        <v>2.281897726883607</v>
       </c>
       <c r="D36" t="n">
-        <v>9.144787586994925</v>
+        <v>2.728461279053791</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.5783671498667829</v>
+        <v>-0.1670834479155833</v>
       </c>
       <c r="F36" t="n">
-        <v>0.56400811029015</v>
+        <v>0.8675606007632086</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1462,19 +1462,19 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.48241045137295</v>
+        <v>10.47573383894938</v>
       </c>
       <c r="C37" t="n">
-        <v>10.4594990597563</v>
+        <v>10.44927461279674</v>
       </c>
       <c r="D37" t="n">
-        <v>4.219296377798996</v>
+        <v>4.87266026219555</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2718091554443798</v>
+        <v>0.3100942002435025</v>
       </c>
       <c r="F37" t="n">
-        <v>0.7861236391961248</v>
+        <v>0.756907086728937</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1490,19 +1490,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.959495247718891</v>
+        <v>5.926155025455974</v>
       </c>
       <c r="C38" t="n">
-        <v>5.889417395384815</v>
+        <v>5.863978782794767</v>
       </c>
       <c r="D38" t="n">
-        <v>7.810887972192197</v>
+        <v>7.021711436949474</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5031812588855704</v>
+        <v>0.4468589795341899</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6155175818822256</v>
+        <v>0.6555854412591077</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1518,19 +1518,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9122236200008085</v>
+        <v>0.8789078211958062</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9557828746555302</v>
+        <v>0.9493639625055781</v>
       </c>
       <c r="D39" t="n">
-        <v>11.59371261023261</v>
+        <v>23.25616703057953</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.7468726893975748</v>
+        <v>-1.480013407055682</v>
       </c>
       <c r="F39" t="n">
-        <v>0.4562404572958972</v>
+        <v>0.1409834876151632</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1546,19 +1546,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-4.246024440364211</v>
+        <v>-4.25074931790132</v>
       </c>
       <c r="C40" t="n">
-        <v>-4.272389160813397</v>
+        <v>-4.2857115391347</v>
       </c>
       <c r="D40" t="n">
-        <v>2.611479572594593</v>
+        <v>3.427842277026373</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1682328031806734</v>
+        <v>0.2181465467030956</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8666127629070691</v>
+        <v>0.827600418791977</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1574,19 +1574,19 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.399537896289476</v>
+        <v>2.361881202990979</v>
       </c>
       <c r="C41" t="n">
-        <v>2.615481501607051</v>
+        <v>2.561603765003468</v>
       </c>
       <c r="D41" t="n">
-        <v>14.62089600582008</v>
+        <v>13.96782388249994</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.9418853380608347</v>
+        <v>-0.8889068687161604</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3479791282229356</v>
+        <v>0.3757390035996983</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
@@ -1602,19 +1602,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.53467826582806</v>
+        <v>10.5340932670329</v>
       </c>
       <c r="C42" t="n">
-        <v>10.52785832041014</v>
+        <v>10.5131804703762</v>
       </c>
       <c r="D42" t="n">
-        <v>1.454023263255139</v>
+        <v>4.415196103329834</v>
       </c>
       <c r="E42" t="n">
-        <v>0.09253347385056314</v>
+        <v>0.2757289082783123</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9263902541305575</v>
+        <v>0.7831274508291599</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1630,22 +1630,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>6.018570300320664</v>
+        <v>6.021736078727709</v>
       </c>
       <c r="C43" t="n">
-        <v>5.943542266852779</v>
+        <v>5.927590230286141</v>
       </c>
       <c r="D43" t="n">
-        <v>9.145236844479376</v>
+        <v>11.40517743093315</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5819993089459587</v>
+        <v>0.712253102275561</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5615012445702342</v>
+        <v>0.4775413736618551</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
         <v>2015</v>
@@ -1658,19 +1658,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9953619466772416</v>
+        <v>0.9413728102545673</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9614970396226129</v>
+        <v>0.9551365489270751</v>
       </c>
       <c r="D44" t="n">
-        <v>8.172857480881108</v>
+        <v>4.172158587682555</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5201174651762012</v>
+        <v>-0.2605512202907825</v>
       </c>
       <c r="F44" t="n">
-        <v>0.603707629513682</v>
+        <v>0.7948617143203816</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-4.557257529927539</v>
+        <v>-4.4969976086772</v>
       </c>
       <c r="C45" t="n">
-        <v>-4.668177890201437</v>
+        <v>-4.642918564831869</v>
       </c>
       <c r="D45" t="n">
-        <v>9.391931559907597</v>
+        <v>12.80749286793569</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5976988645005551</v>
+        <v>0.7998276732476015</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5509681665630712</v>
+        <v>0.4251170582752428</v>
       </c>
       <c r="G45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
         <v>2015</v>
@@ -1714,19 +1714,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.574653801191209</v>
+        <v>2.508976499817244</v>
       </c>
       <c r="C46" t="n">
-        <v>2.588045373273864</v>
+        <v>2.527010746715529</v>
       </c>
       <c r="D46" t="n">
-        <v>1.032808678889809</v>
+        <v>1.474288090189691</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.06572754184601733</v>
+        <v>-0.09206926172297218</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9476824700282682</v>
+        <v>0.9267748784246326</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -1742,19 +1742,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.59668476642354</v>
+        <v>10.54689184103251</v>
       </c>
       <c r="C47" t="n">
-        <v>10.60191466941132</v>
+        <v>10.56509433194383</v>
       </c>
       <c r="D47" t="n">
-        <v>1.01972406641728</v>
+        <v>3.640679158089145</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.05989522720656087</v>
+        <v>-0.2043326109710727</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9523310973343649</v>
+        <v>0.8384471130513453</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -1770,19 +1770,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6.085096833259739</v>
+        <v>6.015089110768668</v>
       </c>
       <c r="C48" t="n">
-        <v>6.127050493752438</v>
+        <v>6.048273514622341</v>
       </c>
       <c r="D48" t="n">
-        <v>5.228246171010966</v>
+        <v>4.276184203571902</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.3070899301266379</v>
+        <v>-0.2400002431875127</v>
       </c>
       <c r="F48" t="n">
-        <v>0.759252117318842</v>
+        <v>0.8107323524793483</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1798,19 +1798,19 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.9771317506091897</v>
+        <v>0.9735195928058091</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9396668346811998</v>
+        <v>0.8948667033232502</v>
       </c>
       <c r="D49" t="n">
-        <v>14.41470136896961</v>
+        <v>34.63109912255605</v>
       </c>
       <c r="E49" t="n">
-        <v>0.8466719988697994</v>
+        <v>1.943665617660186</v>
       </c>
       <c r="F49" t="n">
-        <v>0.3986654379458929</v>
+        <v>0.05429396270406199</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -1826,19 +1826,19 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-4.597813058997881</v>
+        <v>-4.564793454405732</v>
       </c>
       <c r="C50" t="n">
-        <v>-4.515118120630742</v>
+        <v>-4.554095007538647</v>
       </c>
       <c r="D50" t="n">
-        <v>7.10579124036679</v>
+        <v>0.9082010181922225</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.4173707327703671</v>
+        <v>-0.05097265572591816</v>
       </c>
       <c r="F50" t="n">
-        <v>0.6771145869480375</v>
+        <v>0.9594342720768967</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
@@ -1854,19 +1854,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.657614703827844</v>
+        <v>2.547526021952723</v>
       </c>
       <c r="C51" t="n">
-        <v>2.678686335073336</v>
+        <v>2.466072732424143</v>
       </c>
       <c r="D51" t="n">
-        <v>1.709829883302616</v>
+        <v>8.226372147694926</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.1004297659706996</v>
+        <v>0.461703991691612</v>
       </c>
       <c r="F51" t="n">
-        <v>0.9201546873289521</v>
+        <v>0.6451069517048758</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1882,19 +1882,19 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10.73836324580539</v>
+        <v>10.6406952288935</v>
       </c>
       <c r="C52" t="n">
-        <v>10.65006685539413</v>
+        <v>10.56712530102661</v>
       </c>
       <c r="D52" t="n">
-        <v>17.55392155718831</v>
+        <v>15.17120697899201</v>
       </c>
       <c r="E52" t="n">
-        <v>0.8599630159990657</v>
+        <v>0.6436598000177954</v>
       </c>
       <c r="F52" t="n">
-        <v>0.3921656828114156</v>
+        <v>0.5220231622551623</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -1910,22 +1910,22 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>5.989743211503313</v>
+        <v>5.74306470046045</v>
       </c>
       <c r="C53" t="n">
-        <v>5.955417152935073</v>
+        <v>5.933000312372342</v>
       </c>
       <c r="D53" t="n">
-        <v>4.000737185714197</v>
+        <v>21.64974383372853</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1959952939995633</v>
+        <v>-0.9185208405468651</v>
       </c>
       <c r="F53" t="n">
-        <v>0.8451204593155049</v>
+        <v>0.3619091154809978</v>
       </c>
       <c r="G53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
         <v>2017</v>
@@ -1938,19 +1938,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1.049421545455431</v>
+        <v>0.8753415827505295</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9745060217859275</v>
+        <v>0.9874839670141365</v>
       </c>
       <c r="D54" t="n">
-        <v>14.98385079473149</v>
+        <v>54.56348525052551</v>
       </c>
       <c r="E54" t="n">
-        <v>0.734055776581767</v>
+        <v>-2.314932625549125</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4656161820485321</v>
+        <v>0.0235709720984265</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1966,19 +1966,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-4.33983385800687</v>
+        <v>-4.52145301083139</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.437909592468015</v>
+        <v>-4.2761687729164</v>
       </c>
       <c r="D55" t="n">
-        <v>10.31542385680363</v>
+        <v>26.09253183444534</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5053504985940278</v>
+        <v>-1.10701237190773</v>
       </c>
       <c r="F55" t="n">
-        <v>0.614785342937795</v>
+        <v>0.2739128971628914</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -1994,22 +1994,22 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2.832824404287503</v>
+        <v>2.36327343832227</v>
       </c>
       <c r="C56" t="n">
-        <v>2.896001604570449</v>
+        <v>2.564740525471625</v>
       </c>
       <c r="D56" t="n">
-        <v>4.779955478132232</v>
+        <v>24.97634328323974</v>
       </c>
       <c r="E56" t="n">
-        <v>-0.2341690382929033</v>
+        <v>-1.059656502289314</v>
       </c>
       <c r="F56" t="n">
-        <v>0.8153764491643476</v>
+        <v>0.2932910069051754</v>
       </c>
       <c r="G56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
         <v>2017</v>
@@ -2022,19 +2022,19 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.73209550212109</v>
+        <v>10.65828392273467</v>
       </c>
       <c r="C57" t="n">
-        <v>10.65854977980649</v>
+        <v>10.59100200754607</v>
       </c>
       <c r="D57" t="n">
-        <v>14.17974893276519</v>
+        <v>13.67641608732855</v>
       </c>
       <c r="E57" t="n">
-        <v>0.7831022304773366</v>
+        <v>0.7040366084468966</v>
       </c>
       <c r="F57" t="n">
-        <v>0.4351519722747588</v>
+        <v>0.4830286918960539</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -2050,22 +2050,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6.101464207182762</v>
+        <v>5.942411031996848</v>
       </c>
       <c r="C58" t="n">
-        <v>6.15636456769754</v>
+        <v>6.030798619947424</v>
       </c>
       <c r="D58" t="n">
-        <v>6.096887235950424</v>
+        <v>10.35547096773964</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.336711603010767</v>
+        <v>-0.5330804950978804</v>
       </c>
       <c r="F58" t="n">
-        <v>0.7369285138841576</v>
+        <v>0.5951176857196879</v>
       </c>
       <c r="G58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
         <v>2018</v>
@@ -2078,19 +2078,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.193539584552961</v>
+        <v>1.017553850942127</v>
       </c>
       <c r="C59" t="n">
-        <v>1.106109955652392</v>
+        <v>1.066185339879952</v>
       </c>
       <c r="D59" t="n">
-        <v>15.37286771840096</v>
+        <v>15.98575755264627</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8489943690960122</v>
+        <v>-0.8229172364276774</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3982814956537148</v>
+        <v>0.4124740442396625</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2106,19 +2106,19 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-4.718514302826229</v>
+        <v>-4.850086048435441</v>
       </c>
       <c r="C60" t="n">
-        <v>-4.906488624161423</v>
+        <v>-4.695074586199489</v>
       </c>
       <c r="D60" t="n">
-        <v>12.09481487939683</v>
+        <v>10.82017301268639</v>
       </c>
       <c r="E60" t="n">
-        <v>0.6679579838949309</v>
+        <v>-0.5570024970005405</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5056201038525776</v>
+        <v>0.5787868245213592</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
@@ -2134,19 +2134,19 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.854853126466251</v>
+        <v>2.483840838096651</v>
       </c>
       <c r="C61" t="n">
-        <v>2.79398611983693</v>
+        <v>2.557780181611024</v>
       </c>
       <c r="D61" t="n">
-        <v>4.511455880813097</v>
+        <v>7.568128243051894</v>
       </c>
       <c r="E61" t="n">
-        <v>0.249153294583466</v>
+        <v>-0.3895932462501004</v>
       </c>
       <c r="F61" t="n">
-        <v>0.803669109636034</v>
+        <v>0.6976784749377333</v>
       </c>
       <c r="G61" t="b">
         <v>1</v>
@@ -2162,19 +2162,19 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10.79839271553016</v>
+        <v>10.76853029601412</v>
       </c>
       <c r="C62" t="n">
-        <v>10.88636647851982</v>
+        <v>10.85492551419171</v>
       </c>
       <c r="D62" t="n">
-        <v>17.51873359267034</v>
+        <v>17.40404042914625</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.9434126760881332</v>
+        <v>-0.9126755797999814</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3474975411935338</v>
+        <v>0.3634820922443704</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2190,19 +2190,19 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>6.100189458613614</v>
+        <v>6.049599676824356</v>
       </c>
       <c r="C63" t="n">
-        <v>5.928017145247848</v>
+        <v>5.874087797432606</v>
       </c>
       <c r="D63" t="n">
-        <v>15.6815636891267</v>
+        <v>15.92603437192382</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8444780489952342</v>
+        <v>0.8351682882767834</v>
       </c>
       <c r="F63" t="n">
-        <v>0.4001718983939448</v>
+        <v>0.4054673379055376</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2218,19 +2218,19 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.185227990036963</v>
+        <v>1.154672787286548</v>
       </c>
       <c r="C64" t="n">
-        <v>1.136780430519192</v>
+        <v>1.121746277797028</v>
       </c>
       <c r="D64" t="n">
-        <v>15.34846461189549</v>
+        <v>10.84300206622972</v>
       </c>
       <c r="E64" t="n">
-        <v>0.8265401147152894</v>
+        <v>0.5686118253894482</v>
       </c>
       <c r="F64" t="n">
-        <v>0.4103631493447627</v>
+        <v>0.570882135021178</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -2246,19 +2246,19 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-4.726792153276239</v>
+        <v>-4.783899943582421</v>
       </c>
       <c r="C65" t="n">
-        <v>-5.176148458535523</v>
+        <v>-5.254762374471528</v>
       </c>
       <c r="D65" t="n">
-        <v>31.33677741854512</v>
+        <v>32.68065442456593</v>
       </c>
       <c r="E65" t="n">
-        <v>1.687537109233564</v>
+        <v>1.713787976223788</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0944914371721062</v>
+        <v>0.0897075046758606</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2274,22 +2274,22 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2.89832919103753</v>
+        <v>2.828712953199084</v>
       </c>
       <c r="C66" t="n">
-        <v>2.755727279122699</v>
+        <v>2.735063726230522</v>
       </c>
       <c r="D66" t="n">
-        <v>12.69756988854078</v>
+        <v>8.360763223422707</v>
       </c>
       <c r="E66" t="n">
-        <v>0.683785064999006</v>
+        <v>0.4384421223090665</v>
       </c>
       <c r="F66" t="n">
-        <v>0.4955084437672063</v>
+        <v>0.66194308572255</v>
       </c>
       <c r="G66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" t="n">
         <v>2019</v>

</xml_diff>

<commit_message>
Further tighten PSM caliper to 0.01 for very strict matching
Changes:
- Reduced caliper from 0.02 to 0.01 for ultra-strict matching
- Significantly higher match quality with minimal propensity score differences
- Trade-off: substantial sample loss (1544 vs 1732) for precision

Results with caliper=0.01:
- Total matched samples: 1,544 (vs 1,732 with caliper=0.02)
- Average match rate: 75.4% (vs 84.8%)
- Average standardized bias:
  * financial_development: 7.33% (EXCELLENT, <10%)
  * ln_pgdp: 10.09%
  * ln_pop_density: 11.73%
  * ln_fdi_openness: 12.76%
  * industrial_advanced: 16.26%
- 1/5 variables pass <10% threshold

Notable: Year 2015 achieved perfect balance (5/5 variables <10%)
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -482,19 +482,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.831061709726443</v>
+        <v>9.736912990408255</v>
       </c>
       <c r="C2" t="n">
-        <v>9.793361061724081</v>
+        <v>9.795110498754491</v>
       </c>
       <c r="D2" t="n">
-        <v>6.506870464907174</v>
+        <v>9.970030995657181</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3680841784030661</v>
+        <v>-0.5228328362387957</v>
       </c>
       <c r="F2" t="n">
-        <v>0.713432102243335</v>
+        <v>0.6021615488184514</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -510,19 +510,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.896404323736572</v>
+        <v>5.779360639493638</v>
       </c>
       <c r="C3" t="n">
-        <v>5.53742500803248</v>
+        <v>5.544211435638456</v>
       </c>
       <c r="D3" t="n">
-        <v>38.63978847710614</v>
+        <v>24.59983449953187</v>
       </c>
       <c r="E3" t="n">
-        <v>2.185796516462045</v>
+        <v>1.290026204331519</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03067944459355844</v>
+        <v>0.1998060097998725</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8343211364355647</v>
+        <v>0.8149817917992487</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8611218509132418</v>
+        <v>0.8380155618495032</v>
       </c>
       <c r="D4" t="n">
-        <v>9.554165115143155</v>
+        <v>8.912165757529696</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.5404651953194941</v>
+        <v>-0.4673579151428093</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5898306191154187</v>
+        <v>0.6412481536424888</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-4.007612164593573</v>
+        <v>-4.154322749666555</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.341957496718453</v>
+        <v>-4.305347168370659</v>
       </c>
       <c r="D5" t="n">
-        <v>29.47762433334325</v>
+        <v>13.34703078153155</v>
       </c>
       <c r="E5" t="n">
-        <v>1.667506244750128</v>
+        <v>0.6999241990234834</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09838273182892644</v>
+        <v>0.4857721715828911</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -594,19 +594,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.832194796766036</v>
+        <v>1.720043740858602</v>
       </c>
       <c r="C6" t="n">
-        <v>1.880197441810711</v>
+        <v>1.6998600004285</v>
       </c>
       <c r="D6" t="n">
-        <v>5.383435601501279</v>
+        <v>2.617868156811237</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3045331055922108</v>
+        <v>0.1372821643103255</v>
       </c>
       <c r="F6" t="n">
-        <v>0.761232559759102</v>
+        <v>0.8910682800597497</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.893568607345104</v>
+        <v>9.824112266597565</v>
       </c>
       <c r="C7" t="n">
-        <v>9.829904583490093</v>
+        <v>9.785690792334643</v>
       </c>
       <c r="D7" t="n">
-        <v>12.05489296821627</v>
+        <v>7.352848153090739</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7182531433184142</v>
+        <v>0.4093892591207916</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4738078940923257</v>
+        <v>0.6829775617132271</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>2008</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.830136567026361</v>
+        <v>5.748899909517434</v>
       </c>
       <c r="C8" t="n">
-        <v>5.850878607499658</v>
+        <v>5.80651914533559</v>
       </c>
       <c r="D8" t="n">
-        <v>2.621587344944157</v>
+        <v>7.193109493138024</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.156199093260679</v>
+        <v>-0.4004953869382821</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8761089170022287</v>
+        <v>0.6895127481914225</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -678,19 +678,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8160652605894007</v>
+        <v>0.8008101061833253</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7640367752147221</v>
+        <v>0.7555209466439339</v>
       </c>
       <c r="D9" t="n">
-        <v>23.12300236666415</v>
+        <v>19.38167319745432</v>
       </c>
       <c r="E9" t="n">
-        <v>1.377711869910789</v>
+        <v>1.079125893208039</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1704953540543297</v>
+        <v>0.2826671957173535</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -706,22 +706,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4.079403587289681</v>
+        <v>-4.167057331848538</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.047832342663729</v>
+        <v>-4.049212005858351</v>
       </c>
       <c r="D10" t="n">
-        <v>3.199347790857023</v>
+        <v>11.74957519749776</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1906231447604385</v>
+        <v>-0.6541886606301952</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8491577031926544</v>
+        <v>0.514475586630511</v>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>2008</v>
@@ -734,19 +734,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.922261466366433</v>
+        <v>1.733242996343761</v>
       </c>
       <c r="C11" t="n">
-        <v>2.025413593517064</v>
+        <v>1.781638459242064</v>
       </c>
       <c r="D11" t="n">
-        <v>9.930846619091945</v>
+        <v>5.92148491812928</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.5916984761940419</v>
+        <v>-0.3296943270219566</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5550584514864572</v>
+        <v>0.7422348578763185</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -762,22 +762,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.902065307870203</v>
+        <v>9.83023951738442</v>
       </c>
       <c r="C12" t="n">
-        <v>9.939595678788933</v>
+        <v>9.91676270939851</v>
       </c>
       <c r="D12" t="n">
-        <v>6.918364337051003</v>
+        <v>16.28271515475884</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.4004292859989141</v>
+        <v>-0.8992423361216877</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6894900908258059</v>
+        <v>0.3703251629058292</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>2009</v>
@@ -790,19 +790,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.729139006306387</v>
+        <v>5.643622026871703</v>
       </c>
       <c r="C13" t="n">
-        <v>5.838702428465379</v>
+        <v>5.793822832076875</v>
       </c>
       <c r="D13" t="n">
-        <v>13.53612219654284</v>
+        <v>18.96561721464204</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.7834597142170922</v>
+        <v>-1.047410445247515</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4348373488259066</v>
+        <v>0.2970907740258894</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8366142252361952</v>
+        <v>0.8307948046889319</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7900212143625021</v>
+        <v>0.7867696410152358</v>
       </c>
       <c r="D14" t="n">
-        <v>21.47404143716593</v>
+        <v>21.31522885823969</v>
       </c>
       <c r="E14" t="n">
-        <v>1.242900006601959</v>
+        <v>1.177171989516128</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2161509537101326</v>
+        <v>0.2414799952045849</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -846,22 +846,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-4.208259657959464</v>
+        <v>-4.302175702230532</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.311127024150943</v>
+        <v>-4.349475307305727</v>
       </c>
       <c r="D15" t="n">
-        <v>10.28803810182849</v>
+        <v>4.739973284809725</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5954632555822909</v>
+        <v>0.2617735807127319</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5525822864267149</v>
+        <v>0.7939595836500943</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>2009</v>
@@ -874,19 +874,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.003679992214923</v>
+        <v>1.925891811586505</v>
       </c>
       <c r="C16" t="n">
-        <v>2.04696325794343</v>
+        <v>1.887539900214619</v>
       </c>
       <c r="D16" t="n">
-        <v>4.225096485968105</v>
+        <v>4.39144334598628</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.2445451391005945</v>
+        <v>0.2425253857147162</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8072104774265709</v>
+        <v>0.8087930238907631</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.07142485723458</v>
+        <v>10.01234574669279</v>
       </c>
       <c r="C17" t="n">
-        <v>10.04600262706136</v>
+        <v>10.02332015617577</v>
       </c>
       <c r="D17" t="n">
-        <v>4.897239080105492</v>
+        <v>2.171826372398367</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2978874237837781</v>
+        <v>-0.1257035393403102</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7662164051941887</v>
+        <v>0.9001582823793985</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.825947485097656</v>
+        <v>5.728946540637144</v>
       </c>
       <c r="C18" t="n">
-        <v>5.740545715147354</v>
+        <v>5.692770293066534</v>
       </c>
       <c r="D18" t="n">
-        <v>8.907592211278009</v>
+        <v>3.851990278945593</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5418276813793813</v>
+        <v>0.222950056101038</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5887683735682281</v>
+        <v>0.8239280544845839</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -958,22 +958,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8181311529903835</v>
+        <v>0.8138149569137814</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8014471342338714</v>
+        <v>0.7754660955023114</v>
       </c>
       <c r="D19" t="n">
-        <v>5.951004605254284</v>
+        <v>13.87773235697059</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3619854783047291</v>
+        <v>0.8032318317243305</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7179600716403638</v>
+        <v>0.4234656054103143</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>2010</v>
@@ -986,19 +986,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-4.244840813804466</v>
+        <v>-4.28270925911148</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.159135045303332</v>
+        <v>-4.188123805042419</v>
       </c>
       <c r="D20" t="n">
-        <v>7.946893495736044</v>
+        <v>8.617351600191174</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.4833906598813384</v>
+        <v>-0.498765283289057</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6295934618793155</v>
+        <v>0.6188290029075968</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1014,19 +1014,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.064302915813227</v>
+        <v>1.898524817678716</v>
       </c>
       <c r="C21" t="n">
-        <v>2.158606665564263</v>
+        <v>1.934308323858746</v>
       </c>
       <c r="D21" t="n">
-        <v>8.800969493744422</v>
+        <v>4.76302319873701</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.5353420746684626</v>
+        <v>-0.2756798985639291</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5932821427275843</v>
+        <v>0.7832603220620302</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1042,22 +1042,22 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.19344865041129</v>
+        <v>10.15897808157817</v>
       </c>
       <c r="C22" t="n">
-        <v>10.24774486579877</v>
+        <v>10.22754669524996</v>
       </c>
       <c r="D22" t="n">
-        <v>9.387809457322378</v>
+        <v>11.89657248160217</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.567166666320861</v>
+        <v>-0.6885639137462455</v>
       </c>
       <c r="F22" t="n">
-        <v>0.571506889983673</v>
+        <v>0.4923271409017314</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
         <v>2011</v>
@@ -1070,19 +1070,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.79625618531315</v>
+        <v>5.743268295502373</v>
       </c>
       <c r="C23" t="n">
-        <v>5.638520377735698</v>
+        <v>5.622530555302886</v>
       </c>
       <c r="D23" t="n">
-        <v>17.18531091890465</v>
+        <v>12.98082195270666</v>
       </c>
       <c r="E23" t="n">
-        <v>1.038254509518208</v>
+        <v>0.751319388943456</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3008935663962301</v>
+        <v>0.4537978784586014</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1098,22 +1098,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.7874197663375814</v>
+        <v>0.7754292969244182</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8132273906556085</v>
+        <v>0.8074488601431954</v>
       </c>
       <c r="D24" t="n">
-        <v>9.824508954401342</v>
+        <v>11.90496725099189</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.5935499668201146</v>
+        <v>-0.689049796152705</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5538062382025568</v>
+        <v>0.4921016710586021</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>2011</v>
@@ -1126,19 +1126,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-4.243012104507941</v>
+        <v>-4.295466130561967</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.500456033115954</v>
+        <v>-4.506788541550499</v>
       </c>
       <c r="D25" t="n">
-        <v>24.64340600912377</v>
+        <v>19.85893770830503</v>
       </c>
       <c r="E25" t="n">
-        <v>1.488837038770996</v>
+        <v>1.149419119870049</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1388634852498884</v>
+        <v>0.2525678215133185</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1154,19 +1154,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.90400699196487</v>
+        <v>1.82928285014053</v>
       </c>
       <c r="C26" t="n">
-        <v>1.87656195358794</v>
+        <v>1.75265581921467</v>
       </c>
       <c r="D26" t="n">
-        <v>3.064349788811842</v>
+        <v>9.563744069373916</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1851333968869415</v>
+        <v>0.5535417076354987</v>
       </c>
       <c r="F26" t="n">
-        <v>0.853431084434499</v>
+        <v>0.5809705384170916</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1182,19 +1182,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.27469335276085</v>
+        <v>10.24690145859853</v>
       </c>
       <c r="C27" t="n">
-        <v>10.35428343623804</v>
+        <v>10.32307143882102</v>
       </c>
       <c r="D27" t="n">
-        <v>14.62904042815387</v>
+        <v>14.06577401942158</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.9017946166531096</v>
+        <v>-0.8439464411652949</v>
       </c>
       <c r="F27" t="n">
-        <v>0.368639704822749</v>
+        <v>0.4001462705341641</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -1210,22 +1210,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.822736552934555</v>
+        <v>5.781731786291055</v>
       </c>
       <c r="C28" t="n">
-        <v>5.721423620801668</v>
+        <v>5.697005875718966</v>
       </c>
       <c r="D28" t="n">
-        <v>10.85293329125018</v>
+        <v>9.004631686323169</v>
       </c>
       <c r="E28" t="n">
-        <v>0.669019739538708</v>
+        <v>0.54027790117939</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5045249311364384</v>
+        <v>0.5898645279894457</v>
       </c>
       <c r="G28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
         <v>2012</v>
@@ -1238,19 +1238,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8067802742767602</v>
+        <v>0.8071402086010075</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8103035318118849</v>
+        <v>0.791321393671409</v>
       </c>
       <c r="D29" t="n">
-        <v>1.16656591066682</v>
+        <v>5.374245254226277</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.07191195235100803</v>
+        <v>0.3224547152535766</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9427843225540449</v>
+        <v>0.7476443017421767</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.263727066615536</v>
+        <v>-4.327134317446419</v>
       </c>
       <c r="C30" t="n">
-        <v>-4.254713189811389</v>
+        <v>-4.265941568954366</v>
       </c>
       <c r="D30" t="n">
-        <v>0.9473789159710863</v>
+        <v>6.47078741806765</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.05840035855729732</v>
+        <v>-0.388247245084059</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9535189736287069</v>
+        <v>0.6984887985676482</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1294,22 +1294,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.006216308500471</v>
+        <v>1.974044850348537</v>
       </c>
       <c r="C31" t="n">
-        <v>1.91967421242199</v>
+        <v>1.901779557144583</v>
       </c>
       <c r="D31" t="n">
-        <v>10.6512517289047</v>
+        <v>8.917501750742646</v>
       </c>
       <c r="E31" t="n">
-        <v>0.6565872530680763</v>
+        <v>0.5350501050445587</v>
       </c>
       <c r="F31" t="n">
-        <v>0.5124724142717166</v>
+        <v>0.5934705455309353</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
         <v>2012</v>
@@ -1322,19 +1322,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10.38612977746011</v>
+        <v>10.355232513871</v>
       </c>
       <c r="C32" t="n">
-        <v>10.41017709762223</v>
+        <v>10.38017054326086</v>
       </c>
       <c r="D32" t="n">
-        <v>4.875810925575722</v>
+        <v>5.244683434109074</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.2985812212486971</v>
+        <v>-0.3124880803330976</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7656831541579039</v>
+        <v>0.7551379684839833</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1350,19 +1350,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5.905446086039507</v>
+        <v>5.839260382239918</v>
       </c>
       <c r="C33" t="n">
-        <v>5.761157413124963</v>
+        <v>5.7313770112839</v>
       </c>
       <c r="D33" t="n">
-        <v>14.81203018340939</v>
+        <v>11.23297094749528</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9070479001014033</v>
+        <v>0.6692814870372694</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3658743561347727</v>
+        <v>0.5044404787942791</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1378,19 +1378,19 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.8398055093164044</v>
+        <v>0.8285785104056056</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8679561117347987</v>
+        <v>0.8555655234152658</v>
       </c>
       <c r="D34" t="n">
-        <v>9.942134993185444</v>
+        <v>9.769730235136834</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.6088289421793361</v>
+        <v>-0.5820988597129194</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5436163477710321</v>
+        <v>0.5615177248062705</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -1406,19 +1406,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-4.177897145525887</v>
+        <v>-4.22550602748566</v>
       </c>
       <c r="C35" t="n">
-        <v>-4.234198662733117</v>
+        <v>-4.250894070144775</v>
       </c>
       <c r="D35" t="n">
-        <v>5.730914506575491</v>
+        <v>2.551277787347201</v>
       </c>
       <c r="E35" t="n">
-        <v>0.3509454075155996</v>
+        <v>0.1520099178874519</v>
       </c>
       <c r="F35" t="n">
-        <v>0.7261817636988828</v>
+        <v>0.879420837385511</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.248064065886551</v>
+        <v>2.167992712979403</v>
       </c>
       <c r="C36" t="n">
-        <v>2.281897726883607</v>
+        <v>2.169637792311664</v>
       </c>
       <c r="D36" t="n">
-        <v>2.728461279053791</v>
+        <v>0.1513276180288692</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.1670834479155833</v>
+        <v>-0.0090163834392141</v>
       </c>
       <c r="F36" t="n">
-        <v>0.8675606007632086</v>
+        <v>0.992819865420407</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1462,19 +1462,19 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.47573383894938</v>
+        <v>10.4381554158708</v>
       </c>
       <c r="C37" t="n">
-        <v>10.44927461279674</v>
+        <v>10.42646952832905</v>
       </c>
       <c r="D37" t="n">
-        <v>4.87266026219555</v>
+        <v>2.187970738556759</v>
       </c>
       <c r="E37" t="n">
-        <v>0.3100942002435025</v>
+        <v>0.1348755745884566</v>
       </c>
       <c r="F37" t="n">
-        <v>0.756907086728937</v>
+        <v>0.8928976399143003</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1490,19 +1490,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.926155025455974</v>
+        <v>5.883345445145909</v>
       </c>
       <c r="C38" t="n">
-        <v>5.863978782794767</v>
+        <v>5.839421183266503</v>
       </c>
       <c r="D38" t="n">
-        <v>7.021711436949474</v>
+        <v>4.995733155455904</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4468589795341899</v>
+        <v>0.3079576741858877</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6555854412591077</v>
+        <v>0.7585436091792744</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1518,19 +1518,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.8789078211958062</v>
+        <v>0.8795989292121568</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9493639625055781</v>
+        <v>0.9321999214098099</v>
       </c>
       <c r="D39" t="n">
-        <v>23.25616703057953</v>
+        <v>18.1436511653497</v>
       </c>
       <c r="E39" t="n">
-        <v>-1.480013407055682</v>
+        <v>-1.11844977308666</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1409834876151632</v>
+        <v>0.2652375534574049</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1546,19 +1546,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-4.25074931790132</v>
+        <v>-4.324770816880025</v>
       </c>
       <c r="C40" t="n">
-        <v>-4.2857115391347</v>
+        <v>-4.276869555480315</v>
       </c>
       <c r="D40" t="n">
-        <v>3.427842277026373</v>
+        <v>4.816359120068565</v>
       </c>
       <c r="E40" t="n">
-        <v>0.2181465467030956</v>
+        <v>-0.29690031603078</v>
       </c>
       <c r="F40" t="n">
-        <v>0.827600418791977</v>
+        <v>0.7669663868589087</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1574,22 +1574,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.361881202990979</v>
+        <v>2.371459217074209</v>
       </c>
       <c r="C41" t="n">
-        <v>2.561603765003468</v>
+        <v>2.485769935918543</v>
       </c>
       <c r="D41" t="n">
-        <v>13.96782388249994</v>
+        <v>8.29165200630859</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.8889068687161604</v>
+        <v>-0.5111317573543448</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3757390035996983</v>
+        <v>0.6101619661568713</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
         <v>2014</v>
@@ -1602,19 +1602,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.5340932670329</v>
+        <v>10.47817070251551</v>
       </c>
       <c r="C42" t="n">
-        <v>10.5131804703762</v>
+        <v>10.477615455367</v>
       </c>
       <c r="D42" t="n">
-        <v>4.415196103329834</v>
+        <v>0.1196177288518085</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2757289082783123</v>
+        <v>0.007076680273604758</v>
       </c>
       <c r="F42" t="n">
-        <v>0.7831274508291599</v>
+        <v>0.9943638937820353</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1630,22 +1630,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>6.021736078727709</v>
+        <v>5.929667581732782</v>
       </c>
       <c r="C43" t="n">
-        <v>5.927590230286141</v>
+        <v>5.912658457271749</v>
       </c>
       <c r="D43" t="n">
-        <v>11.40517743093315</v>
+        <v>2.068922314586567</v>
       </c>
       <c r="E43" t="n">
-        <v>0.712253102275561</v>
+        <v>0.1223990947812925</v>
       </c>
       <c r="F43" t="n">
-        <v>0.4775413736618551</v>
+        <v>0.9027825958938613</v>
       </c>
       <c r="G43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
         <v>2015</v>
@@ -1658,19 +1658,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9413728102545673</v>
+        <v>0.9285047590605662</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9551365489270751</v>
+        <v>0.9319010345310698</v>
       </c>
       <c r="D44" t="n">
-        <v>4.172158587682555</v>
+        <v>1.071886312401779</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.2605512202907825</v>
+        <v>-0.06341364942581364</v>
       </c>
       <c r="F44" t="n">
-        <v>0.7948617143203816</v>
+        <v>0.9495460964563598</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -1686,22 +1686,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-4.4969976086772</v>
+        <v>-4.501181789806212</v>
       </c>
       <c r="C45" t="n">
-        <v>-4.642918564831869</v>
+        <v>-4.5892468752523</v>
       </c>
       <c r="D45" t="n">
-        <v>12.80749286793569</v>
+        <v>7.643082580844049</v>
       </c>
       <c r="E45" t="n">
-        <v>0.7998276732476015</v>
+        <v>0.4521708633709232</v>
       </c>
       <c r="F45" t="n">
-        <v>0.4251170582752428</v>
+        <v>0.6518931054956201</v>
       </c>
       <c r="G45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
         <v>2015</v>
@@ -1714,19 +1714,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.508976499817244</v>
+        <v>2.437522580216269</v>
       </c>
       <c r="C46" t="n">
-        <v>2.527010746715529</v>
+        <v>2.350700086459388</v>
       </c>
       <c r="D46" t="n">
-        <v>1.474288090189691</v>
+        <v>8.060876259150442</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.09206926172297218</v>
+        <v>0.4768878707082758</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9267748784246326</v>
+        <v>0.634217098881612</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -1742,22 +1742,22 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.54689184103251</v>
+        <v>10.4669314880324</v>
       </c>
       <c r="C47" t="n">
-        <v>10.56509433194383</v>
+        <v>10.55281217833759</v>
       </c>
       <c r="D47" t="n">
-        <v>3.640679158089145</v>
+        <v>18.2308931581428</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.2043326109710727</v>
+        <v>-0.9115446579071402</v>
       </c>
       <c r="F47" t="n">
-        <v>0.8384471130513453</v>
+        <v>0.36438029263901</v>
       </c>
       <c r="G47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
         <v>2016</v>
@@ -1770,19 +1770,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6.015089110768668</v>
+        <v>5.896276059153709</v>
       </c>
       <c r="C48" t="n">
-        <v>6.048273514622341</v>
+        <v>5.91479878325038</v>
       </c>
       <c r="D48" t="n">
-        <v>4.276184203571902</v>
+        <v>2.465700115247456</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.2400002431875127</v>
+        <v>-0.1232850057623729</v>
       </c>
       <c r="F48" t="n">
-        <v>0.8107323524793483</v>
+        <v>0.9021343906317548</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1798,19 +1798,19 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.9735195928058091</v>
+        <v>0.9452211983106165</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8948667033232502</v>
+        <v>0.8987565828464054</v>
       </c>
       <c r="D49" t="n">
-        <v>34.63109912255605</v>
+        <v>22.55865389053159</v>
       </c>
       <c r="E49" t="n">
-        <v>1.943665617660186</v>
+        <v>1.12793269452658</v>
       </c>
       <c r="F49" t="n">
-        <v>0.05429396270406199</v>
+        <v>0.2621032651481278</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -1826,22 +1826,22 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-4.564793454405732</v>
+        <v>-4.641160833433025</v>
       </c>
       <c r="C50" t="n">
-        <v>-4.554095007538647</v>
+        <v>-4.449916676712674</v>
       </c>
       <c r="D50" t="n">
-        <v>0.9082010181922225</v>
+        <v>17.89153453305392</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.05097265572591816</v>
+        <v>-0.8945767266526961</v>
       </c>
       <c r="F50" t="n">
-        <v>0.9594342720768967</v>
+        <v>0.3734012138106489</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
         <v>2016</v>
@@ -1854,19 +1854,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.547526021952723</v>
+        <v>2.386751178989156</v>
       </c>
       <c r="C51" t="n">
-        <v>2.466072732424143</v>
+        <v>2.380654569550281</v>
       </c>
       <c r="D51" t="n">
-        <v>8.226372147694926</v>
+        <v>0.6931069745647053</v>
       </c>
       <c r="E51" t="n">
-        <v>0.461703991691612</v>
+        <v>0.03465534872823526</v>
       </c>
       <c r="F51" t="n">
-        <v>0.6451069517048758</v>
+        <v>0.9724265548430794</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1882,19 +1882,19 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10.6406952288935</v>
+        <v>10.61458603663467</v>
       </c>
       <c r="C52" t="n">
-        <v>10.56712530102661</v>
+        <v>10.5413472890288</v>
       </c>
       <c r="D52" t="n">
-        <v>15.17120697899201</v>
+        <v>14.95363926773573</v>
       </c>
       <c r="E52" t="n">
-        <v>0.6436598000177954</v>
+        <v>0.5791519584913376</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5220231622551623</v>
+        <v>0.5648660065477813</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -1910,19 +1910,19 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>5.74306470046045</v>
+        <v>5.68987264885059</v>
       </c>
       <c r="C53" t="n">
-        <v>5.933000312372342</v>
+        <v>5.930743952375502</v>
       </c>
       <c r="D53" t="n">
-        <v>21.64974383372853</v>
+        <v>27.53619312095456</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.9185208405468651</v>
+        <v>-1.066472173754083</v>
       </c>
       <c r="F53" t="n">
-        <v>0.3619091154809978</v>
+        <v>0.2913941467336004</v>
       </c>
       <c r="G53" t="b">
         <v>0</v>
@@ -1938,19 +1938,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.8753415827505295</v>
+        <v>0.865672325838885</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9874839670141365</v>
+        <v>0.9789057207138038</v>
       </c>
       <c r="D54" t="n">
-        <v>54.56348525052551</v>
+        <v>54.65254397965349</v>
       </c>
       <c r="E54" t="n">
-        <v>-2.314932625549125</v>
+        <v>-2.116683926610664</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0235709720984265</v>
+        <v>0.03865611231831428</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1966,19 +1966,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-4.52145301083139</v>
+        <v>-4.545824089105571</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.2761687729164</v>
+        <v>-4.294672049218908</v>
       </c>
       <c r="D55" t="n">
-        <v>26.09253183444534</v>
+        <v>26.77700131848492</v>
       </c>
       <c r="E55" t="n">
-        <v>-1.10701237190773</v>
+        <v>-1.037068801678661</v>
       </c>
       <c r="F55" t="n">
-        <v>0.2739128971628914</v>
+        <v>0.3058330883890098</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -1994,19 +1994,19 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2.36327343832227</v>
+        <v>2.254269426948576</v>
       </c>
       <c r="C56" t="n">
-        <v>2.564740525471625</v>
+        <v>2.45593550650204</v>
       </c>
       <c r="D56" t="n">
-        <v>24.97634328323974</v>
+        <v>26.02611756906929</v>
       </c>
       <c r="E56" t="n">
-        <v>-1.059656502289314</v>
+        <v>-1.007987199114416</v>
       </c>
       <c r="F56" t="n">
-        <v>0.2932910069051754</v>
+        <v>0.3181345113001362</v>
       </c>
       <c r="G56" t="b">
         <v>0</v>
@@ -2022,19 +2022,19 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.65828392273467</v>
+        <v>10.65058723882587</v>
       </c>
       <c r="C57" t="n">
-        <v>10.59100200754607</v>
+        <v>10.56363408492131</v>
       </c>
       <c r="D57" t="n">
-        <v>13.67641608732855</v>
+        <v>17.75908149518744</v>
       </c>
       <c r="E57" t="n">
-        <v>0.7040366084468966</v>
+        <v>0.8790296867024099</v>
       </c>
       <c r="F57" t="n">
-        <v>0.4830286918960539</v>
+        <v>0.3816216492497514</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -2050,19 +2050,19 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5.942411031996848</v>
+        <v>5.882843330651637</v>
       </c>
       <c r="C58" t="n">
-        <v>6.030798619947424</v>
+        <v>5.985856384291535</v>
       </c>
       <c r="D58" t="n">
-        <v>10.35547096773964</v>
+        <v>12.18868928461292</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.5330804950978804</v>
+        <v>-0.6033093392847925</v>
       </c>
       <c r="F58" t="n">
-        <v>0.5951176857196879</v>
+        <v>0.5477261200608097</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2078,19 +2078,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.017553850942127</v>
+        <v>0.9976830466560648</v>
       </c>
       <c r="C59" t="n">
-        <v>1.066185339879952</v>
+        <v>1.067446642737379</v>
       </c>
       <c r="D59" t="n">
-        <v>15.98575755264627</v>
+        <v>23.01534534380616</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.8229172364276774</v>
+        <v>-1.13920147347689</v>
       </c>
       <c r="F59" t="n">
-        <v>0.4124740442396625</v>
+        <v>0.2576138474066966</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2106,19 +2106,19 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-4.850086048435441</v>
+        <v>-4.888375526160416</v>
       </c>
       <c r="C60" t="n">
-        <v>-4.695074586199489</v>
+        <v>-4.726057878555187</v>
       </c>
       <c r="D60" t="n">
-        <v>10.82017301268639</v>
+        <v>11.10571448040591</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.5570024970005405</v>
+        <v>-0.5497048213311658</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5787868245213592</v>
+        <v>0.5838795660814666</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
@@ -2134,22 +2134,22 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.483840838096651</v>
+        <v>2.387263461597706</v>
       </c>
       <c r="C61" t="n">
-        <v>2.557780181611024</v>
+        <v>2.50533741574685</v>
       </c>
       <c r="D61" t="n">
-        <v>7.568128243051894</v>
+        <v>12.91455286113016</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.3895932462501004</v>
+        <v>-0.6392377532868085</v>
       </c>
       <c r="F61" t="n">
-        <v>0.6976784749377333</v>
+        <v>0.5243360156899408</v>
       </c>
       <c r="G61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
         <v>2018</v>
@@ -2162,19 +2162,19 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10.76853029601412</v>
+        <v>10.69281332939631</v>
       </c>
       <c r="C62" t="n">
-        <v>10.85492551419171</v>
+        <v>10.74154906087003</v>
       </c>
       <c r="D62" t="n">
-        <v>17.40404042914625</v>
+        <v>10.96867114789387</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.9126755797999814</v>
+        <v>-0.5026476580830181</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3634820922443704</v>
+        <v>0.6165854441672161</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2190,19 +2190,19 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>6.049599676824356</v>
+        <v>5.894625147914251</v>
       </c>
       <c r="C63" t="n">
-        <v>5.874087797432606</v>
+        <v>5.732062543737077</v>
       </c>
       <c r="D63" t="n">
-        <v>15.92603437192382</v>
+        <v>15.38320860408958</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8351682882767834</v>
+        <v>0.7049471785953645</v>
       </c>
       <c r="F63" t="n">
-        <v>0.4054673379055376</v>
+        <v>0.4828414810223596</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2218,22 +2218,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.154672787286548</v>
+        <v>1.117763667860282</v>
       </c>
       <c r="C64" t="n">
-        <v>1.121746277797028</v>
+        <v>1.122069619084492</v>
       </c>
       <c r="D64" t="n">
-        <v>10.84300206622972</v>
+        <v>1.425237488111485</v>
       </c>
       <c r="E64" t="n">
-        <v>0.5686118253894482</v>
+        <v>-0.06531258672559603</v>
       </c>
       <c r="F64" t="n">
-        <v>0.570882135021178</v>
+        <v>0.9480856258073255</v>
       </c>
       <c r="G64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
         <v>2019</v>
@@ -2246,19 +2246,19 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-4.783899943582421</v>
+        <v>-4.854742252128414</v>
       </c>
       <c r="C65" t="n">
-        <v>-5.254762374471528</v>
+        <v>-5.303196786572146</v>
       </c>
       <c r="D65" t="n">
-        <v>32.68065442456593</v>
+        <v>30.28666610322077</v>
       </c>
       <c r="E65" t="n">
-        <v>1.713787976223788</v>
+        <v>1.387909399658624</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0897075046758606</v>
+        <v>0.1692249805012288</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2274,19 +2274,19 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2.828712953199084</v>
+        <v>2.772804433438608</v>
       </c>
       <c r="C66" t="n">
-        <v>2.735063726230522</v>
+        <v>2.736523051264367</v>
       </c>
       <c r="D66" t="n">
-        <v>8.360763223422707</v>
+        <v>2.961202785428353</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4384421223090665</v>
+        <v>0.135699359123395</v>
       </c>
       <c r="F66" t="n">
-        <v>0.66194308572255</v>
+        <v>0.8923918585273402</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Revert to caliper=0.05 for balanced PSM matching
Rationale for choosing caliper=0.05:
- Best balance between sample retention and match quality
- 2/5 variables pass <10% threshold (vs 1/5 with caliper=0.01)
- Higher match rates (85-96% vs 55-94% with caliper=0.01)
- More stable results across all years
- Year 2015 achieves perfect balance (5/5 variables)

Results with caliper=0.05:
- Total matched samples: 1,886 (highest among all settings)
- Average match rate: 94.4%
- Average standardized bias:
  * financial_development: 7.46% (EXCELLENT, <10%)
  * ln_pgdp: 9.15% (EXCELLENT, <10%)
  * ln_pop_density: 12.50%
  * industrial_advanced: 12.21%
  * ln_fdi_openness: 12.98%
- 2/5 variables pass <10% threshold

Recommended for final analysis
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -482,22 +482,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.736912990408255</v>
+        <v>9.866885858537243</v>
       </c>
       <c r="C2" t="n">
-        <v>9.795110498754491</v>
+        <v>9.796858244112498</v>
       </c>
       <c r="D2" t="n">
-        <v>9.970030995657181</v>
+        <v>12.35099877627559</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.5228328362387957</v>
+        <v>0.7358956829870943</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6021615488184514</v>
+        <v>0.4630398185859812</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>2007</v>
@@ -510,19 +510,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.779360639493638</v>
+        <v>5.936590613538837</v>
       </c>
       <c r="C3" t="n">
-        <v>5.544211435638456</v>
+        <v>5.544140453629207</v>
       </c>
       <c r="D3" t="n">
-        <v>24.59983449953187</v>
+        <v>43.45956242412928</v>
       </c>
       <c r="E3" t="n">
-        <v>1.290026204331519</v>
+        <v>2.589402278450299</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1998060097998725</v>
+        <v>0.01063014453517161</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8149817917992487</v>
+        <v>0.867083535175366</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8380155618495032</v>
+        <v>0.8771512619902208</v>
       </c>
       <c r="D4" t="n">
-        <v>8.912165757529696</v>
+        <v>2.939690870118161</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.4673579151428093</v>
+        <v>-0.1751522981924275</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6412481536424888</v>
+        <v>0.8612410819124753</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-4.154322749666555</v>
+        <v>-3.95563786284638</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.305347168370659</v>
+        <v>-4.311539890514882</v>
       </c>
       <c r="D5" t="n">
-        <v>13.34703078153155</v>
+        <v>32.34627326450113</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6999241990234834</v>
+        <v>1.927251656909735</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4857721715828911</v>
+        <v>0.05636921911241014</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -594,19 +594,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.720043740858602</v>
+        <v>1.97459045550319</v>
       </c>
       <c r="C6" t="n">
-        <v>1.6998600004285</v>
+        <v>2.030481192103107</v>
       </c>
       <c r="D6" t="n">
-        <v>2.617868156811237</v>
+        <v>5.51500034149419</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1372821643103255</v>
+        <v>-0.3285940689083077</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8910682800597497</v>
+        <v>0.7429585260453673</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.824112266597565</v>
+        <v>9.941805817671584</v>
       </c>
       <c r="C7" t="n">
-        <v>9.785690792334643</v>
+        <v>9.825528099581071</v>
       </c>
       <c r="D7" t="n">
-        <v>7.352848153090739</v>
+        <v>21.78357253987299</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4093892591207916</v>
+        <v>1.342829595994835</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6829775617132271</v>
+        <v>0.1814004727385762</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>2008</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.748899909517434</v>
+        <v>5.91997438393599</v>
       </c>
       <c r="C8" t="n">
-        <v>5.80651914533559</v>
+        <v>5.847710969680237</v>
       </c>
       <c r="D8" t="n">
-        <v>7.193109493138024</v>
+        <v>8.944868383876276</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.4004953869382821</v>
+        <v>0.5513987192028139</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6895127481914225</v>
+        <v>0.582239286441933</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -678,19 +678,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8008101061833253</v>
+        <v>0.8232495113715774</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7555209466439339</v>
+        <v>0.7718025735245637</v>
       </c>
       <c r="D9" t="n">
-        <v>19.38167319745432</v>
+        <v>22.51015062757064</v>
       </c>
       <c r="E9" t="n">
-        <v>1.079125893208039</v>
+        <v>1.387618877375374</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2826671957173535</v>
+        <v>0.1673124880423143</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -706,22 +706,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4.167057331848538</v>
+        <v>-4.009049540374143</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.049212005858351</v>
+        <v>-4.070772577035275</v>
       </c>
       <c r="D10" t="n">
-        <v>11.74957519749776</v>
+        <v>6.329428013209025</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.6541886606301952</v>
+        <v>0.3901721467540982</v>
       </c>
       <c r="F10" t="n">
-        <v>0.514475586630511</v>
+        <v>0.6970921886852728</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>2008</v>
@@ -734,22 +734,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.733242996343761</v>
+        <v>1.989491080568654</v>
       </c>
       <c r="C11" t="n">
-        <v>1.781638459242064</v>
+        <v>2.166964103316953</v>
       </c>
       <c r="D11" t="n">
-        <v>5.92148491812928</v>
+        <v>15.98590910217347</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.3296943270219566</v>
+        <v>-0.985437619196273</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7422348578763185</v>
+        <v>0.3261027945507792</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>2008</v>
@@ -762,22 +762,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.83023951738442</v>
+        <v>9.944738096578352</v>
       </c>
       <c r="C12" t="n">
-        <v>9.91676270939851</v>
+        <v>9.955446779326929</v>
       </c>
       <c r="D12" t="n">
-        <v>16.28271515475884</v>
+        <v>1.994155829074569</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.8992423361216877</v>
+        <v>-0.1204773828060981</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3703251629058292</v>
+        <v>0.9042744985259052</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>2009</v>
@@ -790,22 +790,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.643622026871703</v>
+        <v>5.796489503933924</v>
       </c>
       <c r="C13" t="n">
-        <v>5.793822832076875</v>
+        <v>5.842874110427214</v>
       </c>
       <c r="D13" t="n">
-        <v>18.96561721464204</v>
+        <v>5.748408457145337</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.047410445247515</v>
+        <v>-0.3472914183134347</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2970907740258894</v>
+        <v>0.7289206274373221</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>2009</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8307948046889319</v>
+        <v>0.8569433889038716</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7867696410152358</v>
+        <v>0.8106163152124527</v>
       </c>
       <c r="D14" t="n">
-        <v>21.31522885823969</v>
+        <v>20.56200810249328</v>
       </c>
       <c r="E14" t="n">
-        <v>1.177171989516128</v>
+        <v>1.242258446059252</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2414799952045849</v>
+        <v>0.2161998651917395</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -846,22 +846,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-4.302175702230532</v>
+        <v>-4.159683577438074</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.349475307305727</v>
+        <v>-4.359373052069835</v>
       </c>
       <c r="D15" t="n">
-        <v>4.739973284809725</v>
+        <v>20.01077250846795</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2617735807127319</v>
+        <v>1.208955420934803</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7939595836500943</v>
+        <v>0.2287226000309382</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>2009</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.925891811586505</v>
+        <v>2.158832244540103</v>
       </c>
       <c r="C16" t="n">
-        <v>1.887539900214619</v>
+        <v>2.298959209997159</v>
       </c>
       <c r="D16" t="n">
-        <v>4.39144334598628</v>
+        <v>11.18736457137918</v>
       </c>
       <c r="E16" t="n">
-        <v>0.2425253857147162</v>
+        <v>-0.6758872021966889</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8087930238907631</v>
+        <v>0.5002935070219086</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>2009</v>
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.01234574669279</v>
+        <v>10.10664326431772</v>
       </c>
       <c r="C17" t="n">
-        <v>10.02332015617577</v>
+        <v>10.06586110991063</v>
       </c>
       <c r="D17" t="n">
-        <v>2.171826372398367</v>
+        <v>7.808137970661496</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1257035393403102</v>
+        <v>0.4907338620342996</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9001582823793985</v>
+        <v>0.6243121683477533</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -930,19 +930,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.728946540637144</v>
+        <v>5.888743636791447</v>
       </c>
       <c r="C18" t="n">
-        <v>5.692770293066534</v>
+        <v>5.792937961206031</v>
       </c>
       <c r="D18" t="n">
-        <v>3.851990278945593</v>
+        <v>9.901858143697098</v>
       </c>
       <c r="E18" t="n">
-        <v>0.222950056101038</v>
+        <v>0.6223221344743468</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8239280544845839</v>
+        <v>0.53464033126795</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -958,19 +958,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8138149569137814</v>
+        <v>0.860177124439055</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7754660955023114</v>
+        <v>0.82069920632513</v>
       </c>
       <c r="D19" t="n">
-        <v>13.87773235697059</v>
+        <v>12.13338441343615</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8032318317243305</v>
+        <v>0.7625713857932582</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4234656054103143</v>
+        <v>0.4468712996905381</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -986,19 +986,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-4.28270925911148</v>
+        <v>-4.155354170038526</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.188123805042419</v>
+        <v>-4.166630380924821</v>
       </c>
       <c r="D20" t="n">
-        <v>8.617351600191174</v>
+        <v>1.041862843259531</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.498765283289057</v>
+        <v>0.06548006435130542</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6188290029075968</v>
+        <v>0.9478832679118407</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1014,22 +1014,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.898524817678716</v>
+        <v>2.232405669788315</v>
       </c>
       <c r="C21" t="n">
-        <v>1.934308323858746</v>
+        <v>2.396404415000481</v>
       </c>
       <c r="D21" t="n">
-        <v>4.76302319873701</v>
+        <v>12.09097168607363</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.2756798985639291</v>
+        <v>-0.7599057872118523</v>
       </c>
       <c r="F21" t="n">
-        <v>0.7832603220620302</v>
+        <v>0.4485574965288163</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>2010</v>
@@ -1042,22 +1042,22 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.15897808157817</v>
+        <v>10.23942163573567</v>
       </c>
       <c r="C22" t="n">
-        <v>10.22754669524996</v>
+        <v>10.28121836673852</v>
       </c>
       <c r="D22" t="n">
-        <v>11.89657248160217</v>
+        <v>7.181212332670568</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.6885639137462455</v>
+        <v>-0.4541797466505959</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4923271409017314</v>
+        <v>0.6503351907619035</v>
       </c>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
         <v>2011</v>
@@ -1070,19 +1070,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.743268295502373</v>
+        <v>5.902029585362802</v>
       </c>
       <c r="C23" t="n">
-        <v>5.622530555302886</v>
+        <v>5.739600370862801</v>
       </c>
       <c r="D23" t="n">
-        <v>12.98082195270666</v>
+        <v>16.97606859693585</v>
       </c>
       <c r="E23" t="n">
-        <v>0.751319388943456</v>
+        <v>1.073660849631524</v>
       </c>
       <c r="F23" t="n">
-        <v>0.4537978784586014</v>
+        <v>0.2846163140505338</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1098,22 +1098,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.7754292969244182</v>
+        <v>0.8133325961855089</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8074488601431954</v>
+        <v>0.8303285509948605</v>
       </c>
       <c r="D24" t="n">
-        <v>11.90496725099189</v>
+        <v>6.369362566271564</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.689049796152705</v>
+        <v>-0.402833859056666</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4921016710586021</v>
+        <v>0.687634710658704</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
         <v>2011</v>
@@ -1126,19 +1126,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-4.295466130561967</v>
+        <v>-4.174946423495506</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.506788541550499</v>
+        <v>-4.426698948148167</v>
       </c>
       <c r="D25" t="n">
-        <v>19.85893770830503</v>
+        <v>24.49731295263824</v>
       </c>
       <c r="E25" t="n">
-        <v>1.149419119870049</v>
+        <v>1.549346109685628</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2525678215133185</v>
+        <v>0.123417816646718</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1154,19 +1154,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.82928285014053</v>
+        <v>2.114114942899765</v>
       </c>
       <c r="C26" t="n">
-        <v>1.75265581921467</v>
+        <v>2.119274320347017</v>
       </c>
       <c r="D26" t="n">
-        <v>9.563744069373916</v>
+        <v>0.423493328247691</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5535417076354987</v>
+        <v>-0.02678406982296055</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5809705384170916</v>
+        <v>0.9786699787735358</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1182,19 +1182,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.24690145859853</v>
+        <v>10.3330699093908</v>
       </c>
       <c r="C27" t="n">
-        <v>10.32307143882102</v>
+        <v>10.39372442806099</v>
       </c>
       <c r="D27" t="n">
-        <v>14.06577401942158</v>
+        <v>10.89484661989024</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.8439464411652949</v>
+        <v>-0.7060667589243397</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4001462705341641</v>
+        <v>0.4811473601913111</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -1210,22 +1210,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.781731786291055</v>
+        <v>5.947867890617655</v>
       </c>
       <c r="C28" t="n">
-        <v>5.697005875718966</v>
+        <v>5.831988881966329</v>
       </c>
       <c r="D28" t="n">
-        <v>9.004631686323169</v>
+        <v>11.82134434152247</v>
       </c>
       <c r="E28" t="n">
-        <v>0.54027790117939</v>
+        <v>0.7661106738399815</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5898645279894457</v>
+        <v>0.4447017110189228</v>
       </c>
       <c r="G28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>2012</v>
@@ -1238,19 +1238,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8071402086010075</v>
+        <v>0.8408123037517883</v>
       </c>
       <c r="C29" t="n">
-        <v>0.791321393671409</v>
+        <v>0.8307227554680235</v>
       </c>
       <c r="D29" t="n">
-        <v>5.374245254226277</v>
+        <v>3.312590331547823</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3224547152535766</v>
+        <v>0.2146803897881437</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7476443017421767</v>
+        <v>0.8303090506243311</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.327134317446419</v>
+        <v>-4.177973982144462</v>
       </c>
       <c r="C30" t="n">
-        <v>-4.265941568954366</v>
+        <v>-4.192713194709146</v>
       </c>
       <c r="D30" t="n">
-        <v>6.47078741806765</v>
+        <v>1.568226673438571</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.388247245084059</v>
+        <v>0.1016327042688212</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6984887985676482</v>
+        <v>0.9191888885993031</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1294,19 +1294,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.974044850348537</v>
+        <v>2.200553102795348</v>
       </c>
       <c r="C31" t="n">
-        <v>1.901779557144583</v>
+        <v>2.163361332334392</v>
       </c>
       <c r="D31" t="n">
-        <v>8.917501750742646</v>
+        <v>3.246519542323875</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5350501050445587</v>
+        <v>0.210398513261148</v>
       </c>
       <c r="F31" t="n">
-        <v>0.5934705455309353</v>
+        <v>0.8336359939302548</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -1322,19 +1322,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10.355232513871</v>
+        <v>10.43251584686971</v>
       </c>
       <c r="C32" t="n">
-        <v>10.38017054326086</v>
+        <v>10.43743124418211</v>
       </c>
       <c r="D32" t="n">
-        <v>5.244683434109074</v>
+        <v>0.9613599798445172</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.3124880803330976</v>
+        <v>-0.0608017437528448</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7551379684839833</v>
+        <v>0.9515945828375385</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1350,19 +1350,19 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5.839260382239918</v>
+        <v>5.958671399571555</v>
       </c>
       <c r="C33" t="n">
-        <v>5.7313770112839</v>
+        <v>5.786809720891723</v>
       </c>
       <c r="D33" t="n">
-        <v>11.23297094749528</v>
+        <v>17.72760261446441</v>
       </c>
       <c r="E33" t="n">
-        <v>0.6692814870372694</v>
+        <v>1.121192034321267</v>
       </c>
       <c r="F33" t="n">
-        <v>0.5044404787942791</v>
+        <v>0.2639271815980185</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1378,22 +1378,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.8285785104056056</v>
+        <v>0.8475464717182144</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8555655234152658</v>
+        <v>0.8785000517825547</v>
       </c>
       <c r="D34" t="n">
-        <v>9.769730235136834</v>
+        <v>10.98974525962402</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.5820988597129194</v>
+        <v>-0.6950525185090075</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5615177248062705</v>
+        <v>0.4880854169020128</v>
       </c>
       <c r="G34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>2013</v>
@@ -1406,22 +1406,22 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-4.22550602748566</v>
+        <v>-4.144654605692573</v>
       </c>
       <c r="C35" t="n">
-        <v>-4.250894070144775</v>
+        <v>-4.243482036992442</v>
       </c>
       <c r="D35" t="n">
-        <v>2.551277787347201</v>
+        <v>10.13731348163677</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1520099178874519</v>
+        <v>0.6411399991420739</v>
       </c>
       <c r="F35" t="n">
-        <v>0.879420837385511</v>
+        <v>0.5224416818255502</v>
       </c>
       <c r="G35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
         <v>2013</v>
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.167992712979403</v>
+        <v>2.299863928968326</v>
       </c>
       <c r="C36" t="n">
-        <v>2.169637792311664</v>
+        <v>2.423903792803384</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1513276180288692</v>
+        <v>9.144787586994925</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.0090163834392141</v>
+        <v>-0.5783671498667829</v>
       </c>
       <c r="F36" t="n">
-        <v>0.992819865420407</v>
+        <v>0.56400811029015</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1462,19 +1462,19 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.4381554158708</v>
+        <v>10.48241045137295</v>
       </c>
       <c r="C37" t="n">
-        <v>10.42646952832905</v>
+        <v>10.4594990597563</v>
       </c>
       <c r="D37" t="n">
-        <v>2.187970738556759</v>
+        <v>4.219296377798996</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1348755745884566</v>
+        <v>0.2718091554443798</v>
       </c>
       <c r="F37" t="n">
-        <v>0.8928976399143003</v>
+        <v>0.7861236391961248</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1490,19 +1490,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.883345445145909</v>
+        <v>5.959495247718891</v>
       </c>
       <c r="C38" t="n">
-        <v>5.839421183266503</v>
+        <v>5.889417395384815</v>
       </c>
       <c r="D38" t="n">
-        <v>4.995733155455904</v>
+        <v>7.810887972192197</v>
       </c>
       <c r="E38" t="n">
-        <v>0.3079576741858877</v>
+        <v>0.5031812588855704</v>
       </c>
       <c r="F38" t="n">
-        <v>0.7585436091792744</v>
+        <v>0.6155175818822256</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1518,19 +1518,19 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.8795989292121568</v>
+        <v>0.9122236200008085</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9321999214098099</v>
+        <v>0.9557828746555302</v>
       </c>
       <c r="D39" t="n">
-        <v>18.1436511653497</v>
+        <v>11.59371261023261</v>
       </c>
       <c r="E39" t="n">
-        <v>-1.11844977308666</v>
+        <v>-0.7468726893975748</v>
       </c>
       <c r="F39" t="n">
-        <v>0.2652375534574049</v>
+        <v>0.4562404572958972</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1546,19 +1546,19 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-4.324770816880025</v>
+        <v>-4.246024440364211</v>
       </c>
       <c r="C40" t="n">
-        <v>-4.276869555480315</v>
+        <v>-4.272389160813397</v>
       </c>
       <c r="D40" t="n">
-        <v>4.816359120068565</v>
+        <v>2.611479572594593</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.29690031603078</v>
+        <v>0.1682328031806734</v>
       </c>
       <c r="F40" t="n">
-        <v>0.7669663868589087</v>
+        <v>0.8666127629070691</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1574,22 +1574,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.371459217074209</v>
+        <v>2.399537896289476</v>
       </c>
       <c r="C41" t="n">
-        <v>2.485769935918543</v>
+        <v>2.615481501607051</v>
       </c>
       <c r="D41" t="n">
-        <v>8.29165200630859</v>
+        <v>14.62089600582008</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.5111317573543448</v>
+        <v>-0.9418853380608347</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6101619661568713</v>
+        <v>0.3479791282229356</v>
       </c>
       <c r="G41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>2014</v>
@@ -1602,19 +1602,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.47817070251551</v>
+        <v>10.53467826582806</v>
       </c>
       <c r="C42" t="n">
-        <v>10.477615455367</v>
+        <v>10.52785832041014</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1196177288518085</v>
+        <v>1.454023263255139</v>
       </c>
       <c r="E42" t="n">
-        <v>0.007076680273604758</v>
+        <v>0.09253347385056314</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9943638937820353</v>
+        <v>0.9263902541305575</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1630,19 +1630,19 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5.929667581732782</v>
+        <v>6.018570300320664</v>
       </c>
       <c r="C43" t="n">
-        <v>5.912658457271749</v>
+        <v>5.943542266852779</v>
       </c>
       <c r="D43" t="n">
-        <v>2.068922314586567</v>
+        <v>9.145236844479376</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1223990947812925</v>
+        <v>0.5819993089459587</v>
       </c>
       <c r="F43" t="n">
-        <v>0.9027825958938613</v>
+        <v>0.5615012445702342</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -1658,19 +1658,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9285047590605662</v>
+        <v>0.9953619466772416</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9319010345310698</v>
+        <v>0.9614970396226129</v>
       </c>
       <c r="D44" t="n">
-        <v>1.071886312401779</v>
+        <v>8.172857480881108</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.06341364942581364</v>
+        <v>0.5201174651762012</v>
       </c>
       <c r="F44" t="n">
-        <v>0.9495460964563598</v>
+        <v>0.603707629513682</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -1686,19 +1686,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-4.501181789806212</v>
+        <v>-4.557257529927539</v>
       </c>
       <c r="C45" t="n">
-        <v>-4.5892468752523</v>
+        <v>-4.668177890201437</v>
       </c>
       <c r="D45" t="n">
-        <v>7.643082580844049</v>
+        <v>9.391931559907597</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4521708633709232</v>
+        <v>0.5976988645005551</v>
       </c>
       <c r="F45" t="n">
-        <v>0.6518931054956201</v>
+        <v>0.5509681665630712</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
@@ -1714,19 +1714,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.437522580216269</v>
+        <v>2.574653801191209</v>
       </c>
       <c r="C46" t="n">
-        <v>2.350700086459388</v>
+        <v>2.588045373273864</v>
       </c>
       <c r="D46" t="n">
-        <v>8.060876259150442</v>
+        <v>1.032808678889809</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4768878707082758</v>
+        <v>-0.06572754184601733</v>
       </c>
       <c r="F46" t="n">
-        <v>0.634217098881612</v>
+        <v>0.9476824700282682</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -1742,22 +1742,22 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.4669314880324</v>
+        <v>10.59668476642354</v>
       </c>
       <c r="C47" t="n">
-        <v>10.55281217833759</v>
+        <v>10.60191466941132</v>
       </c>
       <c r="D47" t="n">
-        <v>18.2308931581428</v>
+        <v>1.01972406641728</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.9115446579071402</v>
+        <v>-0.05989522720656087</v>
       </c>
       <c r="F47" t="n">
-        <v>0.36438029263901</v>
+        <v>0.9523310973343649</v>
       </c>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
         <v>2016</v>
@@ -1770,19 +1770,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5.896276059153709</v>
+        <v>6.085096833259739</v>
       </c>
       <c r="C48" t="n">
-        <v>5.91479878325038</v>
+        <v>6.127050493752438</v>
       </c>
       <c r="D48" t="n">
-        <v>2.465700115247456</v>
+        <v>5.228246171010966</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.1232850057623729</v>
+        <v>-0.3070899301266379</v>
       </c>
       <c r="F48" t="n">
-        <v>0.9021343906317548</v>
+        <v>0.759252117318842</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1798,19 +1798,19 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.9452211983106165</v>
+        <v>0.9771317506091897</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8987565828464054</v>
+        <v>0.9396668346811998</v>
       </c>
       <c r="D49" t="n">
-        <v>22.55865389053159</v>
+        <v>14.41470136896961</v>
       </c>
       <c r="E49" t="n">
-        <v>1.12793269452658</v>
+        <v>0.8466719988697994</v>
       </c>
       <c r="F49" t="n">
-        <v>0.2621032651481278</v>
+        <v>0.3986654379458929</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -1826,22 +1826,22 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-4.641160833433025</v>
+        <v>-4.597813058997881</v>
       </c>
       <c r="C50" t="n">
-        <v>-4.449916676712674</v>
+        <v>-4.515118120630742</v>
       </c>
       <c r="D50" t="n">
-        <v>17.89153453305392</v>
+        <v>7.10579124036679</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.8945767266526961</v>
+        <v>-0.4173707327703671</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3734012138106489</v>
+        <v>0.6771145869480375</v>
       </c>
       <c r="G50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="n">
         <v>2016</v>
@@ -1854,19 +1854,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.386751178989156</v>
+        <v>2.657614703827844</v>
       </c>
       <c r="C51" t="n">
-        <v>2.380654569550281</v>
+        <v>2.678686335073336</v>
       </c>
       <c r="D51" t="n">
-        <v>0.6931069745647053</v>
+        <v>1.709829883302616</v>
       </c>
       <c r="E51" t="n">
-        <v>0.03465534872823526</v>
+        <v>-0.1004297659706996</v>
       </c>
       <c r="F51" t="n">
-        <v>0.9724265548430794</v>
+        <v>0.9201546873289521</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1882,19 +1882,19 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10.61458603663467</v>
+        <v>10.73836324580539</v>
       </c>
       <c r="C52" t="n">
-        <v>10.5413472890288</v>
+        <v>10.65006685539413</v>
       </c>
       <c r="D52" t="n">
-        <v>14.95363926773573</v>
+        <v>17.55392155718831</v>
       </c>
       <c r="E52" t="n">
-        <v>0.5791519584913376</v>
+        <v>0.8599630159990657</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5648660065477813</v>
+        <v>0.3921656828114156</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -1910,22 +1910,22 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>5.68987264885059</v>
+        <v>5.989743211503313</v>
       </c>
       <c r="C53" t="n">
-        <v>5.930743952375502</v>
+        <v>5.955417152935073</v>
       </c>
       <c r="D53" t="n">
-        <v>27.53619312095456</v>
+        <v>4.000737185714197</v>
       </c>
       <c r="E53" t="n">
-        <v>-1.066472173754083</v>
+        <v>0.1959952939995633</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2913941467336004</v>
+        <v>0.8451204593155049</v>
       </c>
       <c r="G53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
         <v>2017</v>
@@ -1938,19 +1938,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.865672325838885</v>
+        <v>1.049421545455431</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9789057207138038</v>
+        <v>0.9745060217859275</v>
       </c>
       <c r="D54" t="n">
-        <v>54.65254397965349</v>
+        <v>14.98385079473149</v>
       </c>
       <c r="E54" t="n">
-        <v>-2.116683926610664</v>
+        <v>0.734055776581767</v>
       </c>
       <c r="F54" t="n">
-        <v>0.03865611231831428</v>
+        <v>0.4656161820485321</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1966,19 +1966,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-4.545824089105571</v>
+        <v>-4.33983385800687</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.294672049218908</v>
+        <v>-4.437909592468015</v>
       </c>
       <c r="D55" t="n">
-        <v>26.77700131848492</v>
+        <v>10.31542385680363</v>
       </c>
       <c r="E55" t="n">
-        <v>-1.037068801678661</v>
+        <v>0.5053504985940278</v>
       </c>
       <c r="F55" t="n">
-        <v>0.3058330883890098</v>
+        <v>0.614785342937795</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
@@ -1994,22 +1994,22 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2.254269426948576</v>
+        <v>2.832824404287503</v>
       </c>
       <c r="C56" t="n">
-        <v>2.45593550650204</v>
+        <v>2.896001604570449</v>
       </c>
       <c r="D56" t="n">
-        <v>26.02611756906929</v>
+        <v>4.779955478132232</v>
       </c>
       <c r="E56" t="n">
-        <v>-1.007987199114416</v>
+        <v>-0.2341690382929033</v>
       </c>
       <c r="F56" t="n">
-        <v>0.3181345113001362</v>
+        <v>0.8153764491643476</v>
       </c>
       <c r="G56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
         <v>2017</v>
@@ -2022,19 +2022,19 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.65058723882587</v>
+        <v>10.73209550212109</v>
       </c>
       <c r="C57" t="n">
-        <v>10.56363408492131</v>
+        <v>10.65854977980649</v>
       </c>
       <c r="D57" t="n">
-        <v>17.75908149518744</v>
+        <v>14.17974893276519</v>
       </c>
       <c r="E57" t="n">
-        <v>0.8790296867024099</v>
+        <v>0.7831022304773366</v>
       </c>
       <c r="F57" t="n">
-        <v>0.3816216492497514</v>
+        <v>0.4351519722747588</v>
       </c>
       <c r="G57" t="b">
         <v>0</v>
@@ -2050,22 +2050,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5.882843330651637</v>
+        <v>6.101464207182762</v>
       </c>
       <c r="C58" t="n">
-        <v>5.985856384291535</v>
+        <v>6.15636456769754</v>
       </c>
       <c r="D58" t="n">
-        <v>12.18868928461292</v>
+        <v>6.096887235950424</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.6033093392847925</v>
+        <v>-0.336711603010767</v>
       </c>
       <c r="F58" t="n">
-        <v>0.5477261200608097</v>
+        <v>0.7369285138841576</v>
       </c>
       <c r="G58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
         <v>2018</v>
@@ -2078,19 +2078,19 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.9976830466560648</v>
+        <v>1.193539584552961</v>
       </c>
       <c r="C59" t="n">
-        <v>1.067446642737379</v>
+        <v>1.106109955652392</v>
       </c>
       <c r="D59" t="n">
-        <v>23.01534534380616</v>
+        <v>15.37286771840096</v>
       </c>
       <c r="E59" t="n">
-        <v>-1.13920147347689</v>
+        <v>0.8489943690960122</v>
       </c>
       <c r="F59" t="n">
-        <v>0.2576138474066966</v>
+        <v>0.3982814956537148</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
@@ -2106,19 +2106,19 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-4.888375526160416</v>
+        <v>-4.718514302826229</v>
       </c>
       <c r="C60" t="n">
-        <v>-4.726057878555187</v>
+        <v>-4.906488624161423</v>
       </c>
       <c r="D60" t="n">
-        <v>11.10571448040591</v>
+        <v>12.09481487939683</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.5497048213311658</v>
+        <v>0.6679579838949309</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5838795660814666</v>
+        <v>0.5056201038525776</v>
       </c>
       <c r="G60" t="b">
         <v>0</v>
@@ -2134,22 +2134,22 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.387263461597706</v>
+        <v>2.854853126466251</v>
       </c>
       <c r="C61" t="n">
-        <v>2.50533741574685</v>
+        <v>2.79398611983693</v>
       </c>
       <c r="D61" t="n">
-        <v>12.91455286113016</v>
+        <v>4.511455880813097</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.6392377532868085</v>
+        <v>0.249153294583466</v>
       </c>
       <c r="F61" t="n">
-        <v>0.5243360156899408</v>
+        <v>0.803669109636034</v>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
         <v>2018</v>
@@ -2162,19 +2162,19 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10.69281332939631</v>
+        <v>10.79839271553016</v>
       </c>
       <c r="C62" t="n">
-        <v>10.74154906087003</v>
+        <v>10.88636647851982</v>
       </c>
       <c r="D62" t="n">
-        <v>10.96867114789387</v>
+        <v>17.51873359267034</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.5026476580830181</v>
+        <v>-0.9434126760881332</v>
       </c>
       <c r="F62" t="n">
-        <v>0.6165854441672161</v>
+        <v>0.3474975411935338</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2190,19 +2190,19 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>5.894625147914251</v>
+        <v>6.100189458613614</v>
       </c>
       <c r="C63" t="n">
-        <v>5.732062543737077</v>
+        <v>5.928017145247848</v>
       </c>
       <c r="D63" t="n">
-        <v>15.38320860408958</v>
+        <v>15.6815636891267</v>
       </c>
       <c r="E63" t="n">
-        <v>0.7049471785953645</v>
+        <v>0.8444780489952342</v>
       </c>
       <c r="F63" t="n">
-        <v>0.4828414810223596</v>
+        <v>0.4001718983939448</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2218,22 +2218,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.117763667860282</v>
+        <v>1.185227990036963</v>
       </c>
       <c r="C64" t="n">
-        <v>1.122069619084492</v>
+        <v>1.136780430519192</v>
       </c>
       <c r="D64" t="n">
-        <v>1.425237488111485</v>
+        <v>15.34846461189549</v>
       </c>
       <c r="E64" t="n">
-        <v>-0.06531258672559603</v>
+        <v>0.8265401147152894</v>
       </c>
       <c r="F64" t="n">
-        <v>0.9480856258073255</v>
+        <v>0.4103631493447627</v>
       </c>
       <c r="G64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="n">
         <v>2019</v>
@@ -2246,19 +2246,19 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-4.854742252128414</v>
+        <v>-4.726792153276239</v>
       </c>
       <c r="C65" t="n">
-        <v>-5.303196786572146</v>
+        <v>-5.176148458535523</v>
       </c>
       <c r="D65" t="n">
-        <v>30.28666610322077</v>
+        <v>31.33677741854512</v>
       </c>
       <c r="E65" t="n">
-        <v>1.387909399658624</v>
+        <v>1.687537109233564</v>
       </c>
       <c r="F65" t="n">
-        <v>0.1692249805012288</v>
+        <v>0.0944914371721062</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2274,22 +2274,22 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2.772804433438608</v>
+        <v>2.89832919103753</v>
       </c>
       <c r="C66" t="n">
-        <v>2.736523051264367</v>
+        <v>2.755727279122699</v>
       </c>
       <c r="D66" t="n">
-        <v>2.961202785428353</v>
+        <v>12.69756988854078</v>
       </c>
       <c r="E66" t="n">
-        <v>0.135699359123395</v>
+        <v>0.683785064999006</v>
       </c>
       <c r="F66" t="n">
-        <v>0.8923918585273402</v>
+        <v>0.4955084437672063</v>
       </c>
       <c r="G66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>2019</v>

</xml_diff>

<commit_message>
Implement 1:2 PSM matching with excellent results
Major improvement: Changed from 1:1 to 1:2 matching (each treated unit matches 2 control units)

Results with 1:2 matching:
- Total matched samples: 3,616 (vs 1,886 with 1:1)
- Average match rate: 92% (stable across years)
- Average standardized bias:
  * financial_development: 4.27% (EXCELLENT, <5%!)
  * ln_pgdp: 7.39% (EXCELLENT, <10%)
  * ln_pop_density: 9.95% (EXCELLENT, <10%)
  * industrial_advanced: 7.29% (EXCELLENT, <10%)
  * ln_fdi_openness: 10.48% (ACCEPTABLE)
- 4/5 variables pass <10% threshold (vs 2/5 with 1:1)

Perfect balance years:
- 2016: 5/5 variables <10% (PERFECT)
- 2018: 5/5 variables <10% (PERFECT)

This is the BEST matching specification - highly recommended for final analysis
</commit_message>
<xml_diff>
--- a/PSM_balance_test_results.xlsx
+++ b/PSM_balance_test_results.xlsx
@@ -482,22 +482,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.866885858537243</v>
+        <v>9.829239725928137</v>
       </c>
       <c r="C2" t="n">
-        <v>9.796858244112498</v>
+        <v>9.787629939988197</v>
       </c>
       <c r="D2" t="n">
-        <v>12.35099877627559</v>
+        <v>7.155733838637756</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7358956829870943</v>
+        <v>0.5813345651844624</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4630398185859812</v>
+        <v>0.56151577684686</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>2007</v>
@@ -510,19 +510,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.936590613538837</v>
+        <v>5.869308005469227</v>
       </c>
       <c r="C3" t="n">
-        <v>5.544140453629207</v>
+        <v>5.691601960609328</v>
       </c>
       <c r="D3" t="n">
-        <v>43.45956242412928</v>
+        <v>20.08376446581675</v>
       </c>
       <c r="E3" t="n">
-        <v>2.589402278450299</v>
+        <v>1.631612738299583</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01063014453517161</v>
+        <v>0.1039625531268559</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.867083535175366</v>
+        <v>0.8356276786122637</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8771512619902208</v>
+        <v>0.8273726125563949</v>
       </c>
       <c r="D4" t="n">
-        <v>2.939690870118161</v>
+        <v>2.716295491110813</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1751522981924275</v>
+        <v>0.2206728888812375</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8612410819124753</v>
+        <v>0.825522181897943</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-3.95563786284638</v>
+        <v>-4.024516290011899</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.311539890514882</v>
+        <v>-4.18125365220827</v>
       </c>
       <c r="D5" t="n">
-        <v>32.34627326450113</v>
+        <v>13.78792361562751</v>
       </c>
       <c r="E5" t="n">
-        <v>1.927251656909735</v>
+        <v>1.12013620973545</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05636921911241014</v>
+        <v>0.2638241740228214</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -594,19 +594,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.97459045550319</v>
+        <v>1.835224346843737</v>
       </c>
       <c r="C6" t="n">
-        <v>2.030481192103107</v>
+        <v>1.866749876211355</v>
       </c>
       <c r="D6" t="n">
-        <v>5.51500034149419</v>
+        <v>3.790350480062278</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3285940689083077</v>
+        <v>-0.3079295286705629</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7429585260453673</v>
+        <v>0.758383253108559</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -622,19 +622,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.941805817671584</v>
+        <v>9.922789338507352</v>
       </c>
       <c r="C7" t="n">
-        <v>9.825528099581071</v>
+        <v>9.858881209684402</v>
       </c>
       <c r="D7" t="n">
-        <v>21.78357253987299</v>
+        <v>11.77313990229046</v>
       </c>
       <c r="E7" t="n">
-        <v>1.342829595994835</v>
+        <v>1.002446740681046</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1814004727385762</v>
+        <v>0.3169779854952446</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -650,19 +650,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.91997438393599</v>
+        <v>5.890940730863804</v>
       </c>
       <c r="C8" t="n">
-        <v>5.847710969680237</v>
+        <v>5.83060811445589</v>
       </c>
       <c r="D8" t="n">
-        <v>8.944868383876276</v>
+        <v>7.151939272786767</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5513987192028139</v>
+        <v>0.6089656857096427</v>
       </c>
       <c r="F8" t="n">
-        <v>0.582239286441933</v>
+        <v>0.5430352638227823</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -678,22 +678,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8232495113715774</v>
+        <v>0.8061150784634978</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7718025735245637</v>
+        <v>0.7855672854298189</v>
       </c>
       <c r="D9" t="n">
-        <v>22.51015062757064</v>
+        <v>8.687689935565727</v>
       </c>
       <c r="E9" t="n">
-        <v>1.387618877375374</v>
+        <v>0.7397301427005951</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1673124880423143</v>
+        <v>0.4600773451724722</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>2008</v>
@@ -706,19 +706,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4.009049540374143</v>
+        <v>-4.016348596291934</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.070772577035275</v>
+        <v>-4.010087101691656</v>
       </c>
       <c r="D10" t="n">
-        <v>6.329428013209025</v>
+        <v>0.626090300770677</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3901721467540982</v>
+        <v>-0.05330966815891462</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6970921886852728</v>
+        <v>0.9575293480687921</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -734,22 +734,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.989491080568654</v>
+        <v>1.884657604312366</v>
       </c>
       <c r="C11" t="n">
-        <v>2.166964103316953</v>
+        <v>1.963263022832397</v>
       </c>
       <c r="D11" t="n">
-        <v>15.98590910217347</v>
+        <v>8.541765137243184</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.985437619196273</v>
+        <v>-0.7273050938455726</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3261027945507792</v>
+        <v>0.4676516397692311</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>2008</v>
@@ -762,19 +762,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.944738096578352</v>
+        <v>9.928550433097779</v>
       </c>
       <c r="C12" t="n">
-        <v>9.955446779326929</v>
+        <v>9.957154752276681</v>
       </c>
       <c r="D12" t="n">
-        <v>1.994155829074569</v>
+        <v>5.096511295274887</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1204773828060981</v>
+        <v>-0.4294396749467124</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9042744985259052</v>
+        <v>0.6679312920935199</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -790,22 +790,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.796489503933924</v>
+        <v>5.763360966186962</v>
       </c>
       <c r="C13" t="n">
-        <v>5.842874110427214</v>
+        <v>5.893929813386631</v>
       </c>
       <c r="D13" t="n">
-        <v>5.748408457145337</v>
+        <v>15.86317263400004</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.3472914183134347</v>
+        <v>-1.336654684918368</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7289206274373221</v>
+        <v>0.1824438989087334</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>2009</v>
@@ -818,19 +818,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8569433889038716</v>
+        <v>0.8468864169633683</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8106163152124527</v>
+        <v>0.7969273195571172</v>
       </c>
       <c r="D14" t="n">
-        <v>20.56200810249328</v>
+        <v>18.90256827103027</v>
       </c>
       <c r="E14" t="n">
-        <v>1.242258446059252</v>
+        <v>1.592758713493923</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2161998651917395</v>
+        <v>0.112389108608293</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -846,22 +846,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-4.159683577438074</v>
+        <v>-4.184018014860469</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.359373052069835</v>
+        <v>-4.269087601909147</v>
       </c>
       <c r="D15" t="n">
-        <v>20.01077250846795</v>
+        <v>8.217616812289883</v>
       </c>
       <c r="E15" t="n">
-        <v>1.208955420934803</v>
+        <v>0.6924287003892662</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2287226000309382</v>
+        <v>0.4892430389228511</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>2009</v>
@@ -874,22 +874,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.158832244540103</v>
+        <v>2.072799903705756</v>
       </c>
       <c r="C16" t="n">
-        <v>2.298959209997159</v>
+        <v>2.114985842251688</v>
       </c>
       <c r="D16" t="n">
-        <v>11.18736457137918</v>
+        <v>4.009608718212093</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.6758872021966889</v>
+        <v>-0.3378556359148878</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5002935070219086</v>
+        <v>0.7357379969047073</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>2009</v>
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.10664326431772</v>
+        <v>10.0865103193604</v>
       </c>
       <c r="C17" t="n">
-        <v>10.06586110991063</v>
+        <v>10.05143260080537</v>
       </c>
       <c r="D17" t="n">
-        <v>7.808137970661496</v>
+        <v>6.800523413912818</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4907338620342996</v>
+        <v>0.5928558864885639</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6243121683477533</v>
+        <v>0.5537252249086284</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -930,22 +930,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5.888743636791447</v>
+        <v>5.841332158433575</v>
       </c>
       <c r="C18" t="n">
-        <v>5.792937961206031</v>
+        <v>5.723648640611456</v>
       </c>
       <c r="D18" t="n">
-        <v>9.901858143697098</v>
+        <v>12.75981168792675</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6223221344743468</v>
+        <v>1.112374593725637</v>
       </c>
       <c r="F18" t="n">
-        <v>0.53464033126795</v>
+        <v>0.2668626350904655</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>2010</v>
@@ -958,22 +958,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.860177124439055</v>
+        <v>0.838686800538599</v>
       </c>
       <c r="C19" t="n">
-        <v>0.82069920632513</v>
+        <v>0.8228356783614238</v>
       </c>
       <c r="D19" t="n">
-        <v>12.13338441343615</v>
+        <v>5.179494691386688</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7625713857932582</v>
+        <v>0.4515378787671993</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4468712996905381</v>
+        <v>0.6519362547536516</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
         <v>2010</v>
@@ -986,19 +986,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-4.155354170038526</v>
+        <v>-4.194252502581665</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.166630380924821</v>
+        <v>-4.285419128233397</v>
       </c>
       <c r="D20" t="n">
-        <v>1.041862843259531</v>
+        <v>8.136275945874649</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06548006435130542</v>
+        <v>0.709304092496568</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9478832679118407</v>
+        <v>0.4787094654553457</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1014,19 +1014,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2.232405669788315</v>
+        <v>2.115082805538701</v>
       </c>
       <c r="C21" t="n">
-        <v>2.396404415000481</v>
+        <v>2.247244868106839</v>
       </c>
       <c r="D21" t="n">
-        <v>12.09097168607363</v>
+        <v>11.60300371960224</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.7599057872118523</v>
+        <v>-1.011526413105454</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4485574965288163</v>
+        <v>0.3126403429341347</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1042,19 +1042,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10.23942163573567</v>
+        <v>10.21642352717392</v>
       </c>
       <c r="C22" t="n">
-        <v>10.28121836673852</v>
+        <v>10.20173607856664</v>
       </c>
       <c r="D22" t="n">
-        <v>7.181212332670568</v>
+        <v>2.727664150123969</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.4541797466505959</v>
+        <v>0.2401274157567274</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6503351907619035</v>
+        <v>0.8103915128350152</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -1070,19 +1070,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.902029585362802</v>
+        <v>5.850008004221119</v>
       </c>
       <c r="C23" t="n">
-        <v>5.739600370862801</v>
+        <v>5.687189283204026</v>
       </c>
       <c r="D23" t="n">
-        <v>16.97606859693585</v>
+        <v>17.85626486532637</v>
       </c>
       <c r="E23" t="n">
-        <v>1.073660849631524</v>
+        <v>1.571959926585388</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2846163140505338</v>
+        <v>0.1169886162647973</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1098,22 +1098,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.8133325961855089</v>
+        <v>0.8025566317832121</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8303285509948605</v>
+        <v>0.8328943441229449</v>
       </c>
       <c r="D24" t="n">
-        <v>6.369362566271564</v>
+        <v>11.44157095611179</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.402833859056666</v>
+        <v>-1.007248222169685</v>
       </c>
       <c r="F24" t="n">
-        <v>0.687634710658704</v>
+        <v>0.3146459962967788</v>
       </c>
       <c r="G24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>2011</v>
@@ -1126,19 +1126,19 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-4.174946423495506</v>
+        <v>-4.201314242854846</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.426698948148167</v>
+        <v>-4.366520833715937</v>
       </c>
       <c r="D25" t="n">
-        <v>24.49731295263824</v>
+        <v>16.03797449310285</v>
       </c>
       <c r="E25" t="n">
-        <v>1.549346109685628</v>
+        <v>1.411888398660102</v>
       </c>
       <c r="F25" t="n">
-        <v>0.123417816646718</v>
+        <v>0.1590541599313769</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1154,19 +1154,19 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.114114942899765</v>
+        <v>2.040558179610713</v>
       </c>
       <c r="C26" t="n">
-        <v>2.119274320347017</v>
+        <v>2.110213082940049</v>
       </c>
       <c r="D26" t="n">
-        <v>0.423493328247691</v>
+        <v>6.496558096000375</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.02678406982296055</v>
+        <v>-0.5719185431370338</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9786699787735358</v>
+        <v>0.5678369982572234</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1182,22 +1182,22 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.3330699093908</v>
+        <v>10.30717224257206</v>
       </c>
       <c r="C27" t="n">
-        <v>10.39372442806099</v>
+        <v>10.32785581602919</v>
       </c>
       <c r="D27" t="n">
-        <v>10.89484661989024</v>
+        <v>3.801793879902147</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.7060667589243397</v>
+        <v>-0.3421614491911931</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4811473601913111</v>
+        <v>0.7324554283933457</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
         <v>2012</v>
@@ -1210,22 +1210,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.947867890617655</v>
+        <v>5.895424445608503</v>
       </c>
       <c r="C28" t="n">
-        <v>5.831988881966329</v>
+        <v>5.845677873024751</v>
       </c>
       <c r="D28" t="n">
-        <v>11.82134434152247</v>
+        <v>5.302083973159051</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7661106738399815</v>
+        <v>0.4771875575843146</v>
       </c>
       <c r="F28" t="n">
-        <v>0.4447017110189228</v>
+        <v>0.6335529303345977</v>
       </c>
       <c r="G28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
         <v>2012</v>
@@ -1238,19 +1238,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8408123037517883</v>
+        <v>0.8276629476503929</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8307227554680235</v>
+        <v>0.8166168705060193</v>
       </c>
       <c r="D29" t="n">
-        <v>3.312590331547823</v>
+        <v>4.152441427420447</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2146803897881437</v>
+        <v>0.3737197284678404</v>
       </c>
       <c r="F29" t="n">
-        <v>0.8303090506243311</v>
+        <v>0.7088670581048901</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1266,22 +1266,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.177973982144462</v>
+        <v>-4.204783861258677</v>
       </c>
       <c r="C30" t="n">
-        <v>-4.192713194709146</v>
+        <v>-4.343258509505957</v>
       </c>
       <c r="D30" t="n">
-        <v>1.568226673438571</v>
+        <v>14.03358281430074</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1016327042688212</v>
+        <v>1.263022453287066</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9191888885993031</v>
+        <v>0.2075596011241665</v>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>2012</v>
@@ -1294,19 +1294,19 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2.200553102795348</v>
+        <v>2.144367416890542</v>
       </c>
       <c r="C31" t="n">
-        <v>2.163361332334392</v>
+        <v>2.137093104948296</v>
       </c>
       <c r="D31" t="n">
-        <v>3.246519542323875</v>
+        <v>0.6701153792304834</v>
       </c>
       <c r="E31" t="n">
-        <v>0.210398513261148</v>
+        <v>0.06031038413074349</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8336359939302548</v>
+        <v>0.9519484865350623</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -1322,19 +1322,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10.43251584686971</v>
+        <v>10.4183439517295</v>
       </c>
       <c r="C32" t="n">
-        <v>10.43743124418211</v>
+        <v>10.44459248749802</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9613599798445172</v>
+        <v>5.055587097592566</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.0608017437528448</v>
+        <v>-0.4450639807773926</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9515945828375385</v>
+        <v>0.6565916854899672</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1350,22 +1350,22 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5.958671399571555</v>
+        <v>5.9138102331517</v>
       </c>
       <c r="C33" t="n">
-        <v>5.786809720891723</v>
+        <v>5.824186381112258</v>
       </c>
       <c r="D33" t="n">
-        <v>17.72760261446441</v>
+        <v>9.399734450066733</v>
       </c>
       <c r="E33" t="n">
-        <v>1.121192034321267</v>
+        <v>0.8274970150527601</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2639271815980185</v>
+        <v>0.4086070023403655</v>
       </c>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
         <v>2013</v>
@@ -1378,22 +1378,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.8475464717182144</v>
+        <v>0.8395363219971425</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8785000517825547</v>
+        <v>0.8308908446481602</v>
       </c>
       <c r="D34" t="n">
-        <v>10.98974525962402</v>
+        <v>3.161677622766176</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.6950525185090075</v>
+        <v>0.2783353943982474</v>
       </c>
       <c r="F34" t="n">
-        <v>0.4880854169020128</v>
+        <v>0.7809489003730228</v>
       </c>
       <c r="G34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
         <v>2013</v>
@@ -1406,19 +1406,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-4.144654605692573</v>
+        <v>-4.172184092911954</v>
       </c>
       <c r="C35" t="n">
-        <v>-4.243482036992442</v>
+        <v>-4.279445823571545</v>
       </c>
       <c r="D35" t="n">
-        <v>10.13731348163677</v>
+        <v>11.02928039492394</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6411399991420739</v>
+        <v>0.9709526001465595</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5224416818255502</v>
+        <v>0.332404367209988</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2.299863928968326</v>
+        <v>2.244598742167236</v>
       </c>
       <c r="C36" t="n">
-        <v>2.423903792803384</v>
+        <v>2.250750552932674</v>
       </c>
       <c r="D36" t="n">
-        <v>9.144787586994925</v>
+        <v>0.5211734407468798</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.5783671498667829</v>
+        <v>-0.04588102662195502</v>
       </c>
       <c r="F36" t="n">
-        <v>0.56400811029015</v>
+        <v>0.963438292346557</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1462,19 +1462,19 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10.48241045137295</v>
+        <v>10.46009141707349</v>
       </c>
       <c r="C37" t="n">
-        <v>10.4594990597563</v>
+        <v>10.4839444215712</v>
       </c>
       <c r="D37" t="n">
-        <v>4.219296377798996</v>
+        <v>4.290519949569704</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2718091554443798</v>
+        <v>-0.3837557706422732</v>
       </c>
       <c r="F37" t="n">
-        <v>0.7861236391961248</v>
+        <v>0.7014339370901093</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1490,19 +1490,19 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5.959495247718891</v>
+        <v>5.908402886581285</v>
       </c>
       <c r="C38" t="n">
-        <v>5.889417395384815</v>
+        <v>5.822171643476388</v>
       </c>
       <c r="D38" t="n">
-        <v>7.810887972192197</v>
+        <v>9.808684113623839</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5031812588855704</v>
+        <v>0.877315377915407</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6155175818822256</v>
+        <v>0.3809804230312244</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1518,22 +1518,22 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9122236200008085</v>
+        <v>0.8890350942936577</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9557828746555302</v>
+        <v>0.902338305514099</v>
       </c>
       <c r="D39" t="n">
-        <v>11.59371261023261</v>
+        <v>3.818577046904329</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.7468726893975748</v>
+        <v>-0.3415439141679393</v>
       </c>
       <c r="F39" t="n">
-        <v>0.4562404572958972</v>
+        <v>0.7329203632558292</v>
       </c>
       <c r="G39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
         <v>2014</v>
@@ -1546,22 +1546,22 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-4.246024440364211</v>
+        <v>-4.268933074147087</v>
       </c>
       <c r="C40" t="n">
-        <v>-4.272389160813397</v>
+        <v>-4.483743122155155</v>
       </c>
       <c r="D40" t="n">
-        <v>2.611479572594593</v>
+        <v>20.01667071145569</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1682328031806734</v>
+        <v>1.79034545576176</v>
       </c>
       <c r="F40" t="n">
-        <v>0.8666127629070691</v>
+        <v>0.07435097083421302</v>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>2014</v>
@@ -1574,22 +1574,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2.399537896289476</v>
+        <v>2.352201950680395</v>
       </c>
       <c r="C41" t="n">
-        <v>2.615481501607051</v>
+        <v>2.328519757969389</v>
       </c>
       <c r="D41" t="n">
-        <v>14.62089600582008</v>
+        <v>1.798933510973164</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.9418853380608347</v>
+        <v>0.1609015047015344</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3479791282229356</v>
+        <v>0.8722900763118506</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
         <v>2014</v>
@@ -1602,19 +1602,19 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10.53467826582806</v>
+        <v>10.53065373694804</v>
       </c>
       <c r="C42" t="n">
-        <v>10.52785832041014</v>
+        <v>10.57373226761539</v>
       </c>
       <c r="D42" t="n">
-        <v>1.454023263255139</v>
+        <v>8.612137869023698</v>
       </c>
       <c r="E42" t="n">
-        <v>0.09253347385056314</v>
+        <v>-0.7702930282694866</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9263902541305575</v>
+        <v>0.4417017399994001</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1630,19 +1630,19 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>6.018570300320664</v>
+        <v>6.001018882496957</v>
       </c>
       <c r="C43" t="n">
-        <v>5.943542266852779</v>
+        <v>5.922019178062795</v>
       </c>
       <c r="D43" t="n">
-        <v>9.145236844479376</v>
+        <v>8.976343996429668</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5819993089459587</v>
+        <v>0.8028686146175545</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5615012445702342</v>
+        <v>0.4226668827318965</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -1658,22 +1658,22 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9953619466772416</v>
+        <v>0.9751950707915051</v>
       </c>
       <c r="C44" t="n">
-        <v>0.9614970396226129</v>
+        <v>0.9362190837327006</v>
       </c>
       <c r="D44" t="n">
-        <v>8.172857480881108</v>
+        <v>10.85426849170125</v>
       </c>
       <c r="E44" t="n">
-        <v>0.5201174651762012</v>
+        <v>0.9708352877391248</v>
       </c>
       <c r="F44" t="n">
-        <v>0.603707629513682</v>
+        <v>0.3323694787362178</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="n">
         <v>2015</v>
@@ -1686,19 +1686,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-4.557257529927539</v>
+        <v>-4.567239864773629</v>
       </c>
       <c r="C45" t="n">
-        <v>-4.668177890201437</v>
+        <v>-4.548838828897362</v>
       </c>
       <c r="D45" t="n">
-        <v>9.391931559907597</v>
+        <v>1.602372446386366</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5976988645005551</v>
+        <v>-0.143320548615702</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5509681665630712</v>
+        <v>0.8861415351921186</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
@@ -1714,19 +1714,19 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2.574653801191209</v>
+        <v>2.536205780781818</v>
       </c>
       <c r="C46" t="n">
-        <v>2.588045373273864</v>
+        <v>2.54589863676282</v>
       </c>
       <c r="D46" t="n">
-        <v>1.032808678889809</v>
+        <v>0.79102416612175</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.06572754184601733</v>
+        <v>-0.07075135229173275</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9476824700282682</v>
+        <v>0.9436430535091106</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -1742,19 +1742,19 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>10.59668476642354</v>
+        <v>10.56680115373898</v>
       </c>
       <c r="C47" t="n">
-        <v>10.60191466941132</v>
+        <v>10.61034212641372</v>
       </c>
       <c r="D47" t="n">
-        <v>1.01972406641728</v>
+        <v>8.805064312646289</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.05989522720656087</v>
+        <v>-0.7098869797889958</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9523310973343649</v>
+        <v>0.4784430208313307</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -1770,19 +1770,19 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6.085096833259739</v>
+        <v>6.03056100833826</v>
       </c>
       <c r="C48" t="n">
-        <v>6.127050493752438</v>
+        <v>6.027205945258892</v>
       </c>
       <c r="D48" t="n">
-        <v>5.228246171010966</v>
+        <v>0.4121055221214463</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.3070899301266379</v>
+        <v>0.0332250093884025</v>
       </c>
       <c r="F48" t="n">
-        <v>0.759252117318842</v>
+        <v>0.9735208548311841</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1798,22 +1798,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.9771317506091897</v>
+        <v>0.9741921494465053</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9396668346811998</v>
+        <v>0.9521731658993424</v>
       </c>
       <c r="D49" t="n">
-        <v>14.41470136896961</v>
+        <v>8.360744347133181</v>
       </c>
       <c r="E49" t="n">
-        <v>0.8466719988697994</v>
+        <v>0.674064758942178</v>
       </c>
       <c r="F49" t="n">
-        <v>0.3986654379458929</v>
+        <v>0.5008761216330022</v>
       </c>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
         <v>2016</v>
@@ -1826,19 +1826,19 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-4.597813058997881</v>
+        <v>-4.586168618374558</v>
       </c>
       <c r="C50" t="n">
-        <v>-4.515118120630742</v>
+        <v>-4.506830958335294</v>
       </c>
       <c r="D50" t="n">
-        <v>7.10579124036679</v>
+        <v>6.874622668098504</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.4173707327703671</v>
+        <v>-0.5542497987250602</v>
       </c>
       <c r="F50" t="n">
-        <v>0.6771145869480375</v>
+        <v>0.5799251531676033</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
@@ -1854,19 +1854,19 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2.657614703827844</v>
+        <v>2.595593221839091</v>
       </c>
       <c r="C51" t="n">
-        <v>2.678686335073336</v>
+        <v>2.587790863679216</v>
       </c>
       <c r="D51" t="n">
-        <v>1.709829883302616</v>
+        <v>0.6945021791234877</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.1004297659706996</v>
+        <v>0.05599255574848565</v>
       </c>
       <c r="F51" t="n">
-        <v>0.9201546873289521</v>
+        <v>0.9553913619441702</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1882,19 +1882,19 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10.73836324580539</v>
+        <v>10.72036828885553</v>
       </c>
       <c r="C52" t="n">
-        <v>10.65006685539413</v>
+        <v>10.66688788917371</v>
       </c>
       <c r="D52" t="n">
-        <v>17.55392155718831</v>
+        <v>10.83454569062315</v>
       </c>
       <c r="E52" t="n">
-        <v>0.8599630159990657</v>
+        <v>0.7268034200868232</v>
       </c>
       <c r="F52" t="n">
-        <v>0.3921656828114156</v>
+        <v>0.4683638189190041</v>
       </c>
       <c r="G52" t="b">
         <v>0</v>
@@ -1910,19 +1910,19 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>5.989743211503313</v>
+        <v>5.936218188188179</v>
       </c>
       <c r="C53" t="n">
-        <v>5.955417152935073</v>
+        <v>5.898967071544707</v>
       </c>
       <c r="D53" t="n">
-        <v>4.000737185714197</v>
+        <v>3.969033460233264</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1959952939995633</v>
+        <v>0.2662508586615836</v>
       </c>
       <c r="F53" t="n">
-        <v>0.8451204593155049</v>
+        <v>0.7903639531051354</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
@@ -1938,19 +1938,19 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1.049421545455431</v>
+        <v>1.030063098897411</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9745060217859275</v>
+        <v>0.9625185158497545</v>
       </c>
       <c r="D54" t="n">
-        <v>14.98385079473149</v>
+        <v>13.76974189313934</v>
       </c>
       <c r="E54" t="n">
-        <v>0.734055776581767</v>
+        <v>0.9237023671705864</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4656161820485321</v>
+        <v>0.3575996130405674</v>
       </c>
       <c r="G54" t="b">
         <v>0</v>
@@ -1966,22 +1966,22 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-4.33983385800687</v>
+        <v>-4.381507147163016</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.437909592468015</v>
+        <v>-4.454712294923715</v>
       </c>
       <c r="D55" t="n">
-        <v>10.31542385680363</v>
+        <v>7.223726843458339</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5053504985940278</v>
+        <v>0.4845823281858848</v>
       </c>
       <c r="F55" t="n">
-        <v>0.614785342937795</v>
+        <v>0.6286374314380718</v>
       </c>
       <c r="G55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
         <v>2017</v>
@@ -1994,19 +1994,19 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2.832824404287503</v>
+        <v>2.709924375681024</v>
       </c>
       <c r="C56" t="n">
-        <v>2.896001604570449</v>
+        <v>2.72050836131125</v>
       </c>
       <c r="D56" t="n">
-        <v>4.779955478132232</v>
+        <v>0.9335252615893032</v>
       </c>
       <c r="E56" t="n">
-        <v>-0.2341690382929033</v>
+        <v>-0.06262277830880866</v>
       </c>
       <c r="F56" t="n">
-        <v>0.8153764491643476</v>
+        <v>0.9501371906257187</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>10.73209550212109</v>
+        <v>10.6876075826532</v>
       </c>
       <c r="C57" t="n">
-        <v>10.65854977980649</v>
+        <v>10.65090309090737</v>
       </c>
       <c r="D57" t="n">
-        <v>14.17974893276519</v>
+        <v>7.576805626996301</v>
       </c>
       <c r="E57" t="n">
-        <v>0.7831022304773366</v>
+        <v>0.5669962148480215</v>
       </c>
       <c r="F57" t="n">
-        <v>0.4351519722747588</v>
+        <v>0.5712956562122783</v>
       </c>
       <c r="G57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" t="n">
         <v>2018</v>
@@ -2050,19 +2050,19 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6.101464207182762</v>
+        <v>6.012465046925876</v>
       </c>
       <c r="C58" t="n">
-        <v>6.15636456769754</v>
+        <v>6.01386083296403</v>
       </c>
       <c r="D58" t="n">
-        <v>6.096887235950424</v>
+        <v>0.1570898694269849</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.336711603010767</v>
+        <v>-0.01175552940657664</v>
       </c>
       <c r="F58" t="n">
-        <v>0.7369285138841576</v>
+        <v>0.9906312321569467</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
@@ -2078,22 +2078,22 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.193539584552961</v>
+        <v>1.114626379088693</v>
       </c>
       <c r="C59" t="n">
-        <v>1.106109955652392</v>
+        <v>1.108809213754528</v>
       </c>
       <c r="D59" t="n">
-        <v>15.37286771840096</v>
+        <v>1.213424751680905</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8489943690960122</v>
+        <v>0.09080439370842386</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3982814956537148</v>
+        <v>0.9277463212896047</v>
       </c>
       <c r="G59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="n">
         <v>2018</v>
@@ -2106,22 +2106,22 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-4.718514302826229</v>
+        <v>-4.767023921402441</v>
       </c>
       <c r="C60" t="n">
-        <v>-4.906488624161423</v>
+        <v>-4.736256106364009</v>
       </c>
       <c r="D60" t="n">
-        <v>12.09481487939683</v>
+        <v>2.122932783884273</v>
       </c>
       <c r="E60" t="n">
-        <v>0.6679579838949309</v>
+        <v>-0.1588657426489031</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5056201038525776</v>
+        <v>0.873929536838558</v>
       </c>
       <c r="G60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
         <v>2018</v>
@@ -2134,19 +2134,19 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.854853126466251</v>
+        <v>2.674739599062816</v>
       </c>
       <c r="C61" t="n">
-        <v>2.79398611983693</v>
+        <v>2.707476950636596</v>
       </c>
       <c r="D61" t="n">
-        <v>4.511455880813097</v>
+        <v>2.74928598062662</v>
       </c>
       <c r="E61" t="n">
-        <v>0.249153294583466</v>
+        <v>-0.2057377239553127</v>
       </c>
       <c r="F61" t="n">
-        <v>0.803669109636034</v>
+        <v>0.8371854543086676</v>
       </c>
       <c r="G61" t="b">
         <v>1</v>
@@ -2162,19 +2162,19 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10.79839271553016</v>
+        <v>10.79641484465381</v>
       </c>
       <c r="C62" t="n">
-        <v>10.88636647851982</v>
+        <v>10.8628693886696</v>
       </c>
       <c r="D62" t="n">
-        <v>17.51873359267034</v>
+        <v>13.51726521598643</v>
       </c>
       <c r="E62" t="n">
-        <v>-0.9434126760881332</v>
+        <v>-1.016045271084974</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3474975411935338</v>
+        <v>0.3107260575669743</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2190,19 +2190,19 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>6.100189458613614</v>
+        <v>6.085463768345218</v>
       </c>
       <c r="C63" t="n">
-        <v>5.928017145247848</v>
+        <v>5.899569786400985</v>
       </c>
       <c r="D63" t="n">
-        <v>15.6815636891267</v>
+        <v>17.63555123540545</v>
       </c>
       <c r="E63" t="n">
-        <v>0.8444780489952342</v>
+        <v>1.325602342589154</v>
       </c>
       <c r="F63" t="n">
-        <v>0.4001718983939448</v>
+        <v>0.1863225685116709</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2218,22 +2218,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>1.185227990036963</v>
+        <v>1.180635106869439</v>
       </c>
       <c r="C64" t="n">
-        <v>1.136780430519192</v>
+        <v>1.190077384058144</v>
       </c>
       <c r="D64" t="n">
-        <v>15.34846461189549</v>
+        <v>2.534679938536959</v>
       </c>
       <c r="E64" t="n">
-        <v>0.8265401147152894</v>
+        <v>-0.1905229737017107</v>
       </c>
       <c r="F64" t="n">
-        <v>0.4103631493447627</v>
+        <v>0.8490732039297572</v>
       </c>
       <c r="G64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
         <v>2019</v>
@@ -2246,19 +2246,19 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-4.726792153276239</v>
+        <v>-4.73579074923142</v>
       </c>
       <c r="C65" t="n">
-        <v>-5.176148458535523</v>
+        <v>-5.097826468618694</v>
       </c>
       <c r="D65" t="n">
-        <v>31.33677741854512</v>
+        <v>26.55350993013897</v>
       </c>
       <c r="E65" t="n">
-        <v>1.687537109233564</v>
+        <v>1.995933923329236</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0944914371721062</v>
+        <v>0.04721616279401685</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2274,19 +2274,19 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2.89832919103753</v>
+        <v>2.880900862416535</v>
       </c>
       <c r="C66" t="n">
-        <v>2.755727279122699</v>
+        <v>2.737875779510547</v>
       </c>
       <c r="D66" t="n">
-        <v>12.69756988854078</v>
+        <v>12.91344591233447</v>
       </c>
       <c r="E66" t="n">
-        <v>0.683785064999006</v>
+        <v>0.9706582983310611</v>
       </c>
       <c r="F66" t="n">
-        <v>0.4955084437672063</v>
+        <v>0.3327749143983104</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>

</xml_diff>